<commit_message>
policy assessment cards and more cleaning
</commit_message>
<xml_diff>
--- a/inputs/all_data_compiled.xlsx
+++ b/inputs/all_data_compiled.xlsx
@@ -1197,6 +1197,12 @@
       <c r="L7">
         <v>0.432902672615501</v>
       </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
       <c r="O7">
         <v>0.389419132506782</v>
       </c>
@@ -1268,6 +1274,12 @@
       <c r="L8">
         <v>0.403793944470449</v>
       </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
       <c r="O8">
         <v>0.339851966509808</v>
       </c>
@@ -1339,6 +1351,12 @@
       <c r="L9">
         <v>0.432902672615501</v>
       </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
       <c r="O9">
         <v>0.362657249688178</v>
       </c>
@@ -1487,6 +1505,12 @@
       <c r="L11">
         <v>0.382118437118437</v>
       </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
       <c r="O11">
         <v>0.188758185279946</v>
       </c>
@@ -1558,6 +1582,12 @@
       <c r="L12">
         <v>0.238984286945568</v>
       </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
       <c r="O12">
         <v>0.379713214478772</v>
       </c>
@@ -1629,6 +1659,12 @@
       <c r="L13">
         <v>0.382118437118437</v>
       </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
       <c r="O13">
         <v>0.423254612246285</v>
       </c>
@@ -1700,6 +1736,12 @@
       <c r="L14">
         <v>0.339605685126709</v>
       </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
       <c r="O14">
         <v>0.215076821856866</v>
       </c>
@@ -1845,6 +1887,12 @@
       <c r="L16">
         <v>0.40868266233886</v>
       </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
       <c r="O16">
         <v>0.421655744050761</v>
       </c>
@@ -1916,6 +1964,12 @@
       <c r="L17">
         <v>0.41525155702608</v>
       </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
       <c r="O17">
         <v>0.409498502939167</v>
       </c>
@@ -1987,6 +2041,12 @@
       <c r="L18">
         <v>0.399510616283393</v>
       </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
       <c r="O18">
         <v>0.31356117758185</v>
       </c>
@@ -2289,6 +2349,12 @@
       <c r="L22">
         <v>0.403793944470449</v>
       </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
       <c r="O22">
         <v>0.414358425287269</v>
       </c>
@@ -2437,6 +2503,12 @@
       <c r="L24">
         <v>0.330754776712315</v>
       </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
       <c r="O24">
         <v>0.211300149506622</v>
       </c>
@@ -2585,6 +2657,12 @@
       <c r="L26">
         <v>0.403793944470449</v>
       </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
       <c r="O26">
         <v>0.390687508315041</v>
       </c>
@@ -2656,6 +2734,12 @@
       <c r="L27">
         <v>0.362780034735979</v>
       </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
       <c r="O27">
         <v>0.459895423958806</v>
       </c>
@@ -2727,6 +2811,12 @@
       <c r="L28">
         <v>0.399510616283393</v>
       </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
       <c r="O28">
         <v>0.366896550573602</v>
       </c>
@@ -2798,6 +2888,12 @@
       <c r="L29">
         <v>0.327049914685371</v>
       </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
       <c r="O29">
         <v>0.288049120682868</v>
       </c>
@@ -2946,6 +3042,12 @@
       <c r="L31">
         <v>0.327049914685371</v>
       </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
       <c r="O31">
         <v>0.341160373719579</v>
       </c>
@@ -3017,6 +3119,12 @@
       <c r="L32">
         <v>0.327049914685371</v>
       </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
       <c r="O32">
         <v>0.25072679164382</v>
       </c>
@@ -3079,6 +3187,12 @@
       <c r="L33">
         <v>0.388003116567215</v>
       </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
       <c r="P33">
         <v>0.191428783823967</v>
       </c>
@@ -3144,6 +3258,12 @@
       <c r="L34">
         <v>0.41525155702608</v>
       </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
       <c r="O34">
         <v>0.249226386447578</v>
       </c>
@@ -3215,6 +3335,12 @@
       <c r="L35">
         <v>0.432902672615501</v>
       </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
       <c r="O35">
         <v>0.388146298892102</v>
       </c>
@@ -3517,6 +3643,12 @@
       <c r="L39">
         <v>0.432902672615501</v>
       </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
       <c r="O39">
         <v>0.382805248991804</v>
       </c>
@@ -4050,6 +4182,12 @@
       <c r="L46">
         <v>0.41525155702608</v>
       </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
       <c r="O46">
         <v>0.342239164554777</v>
       </c>
@@ -4198,6 +4336,12 @@
       <c r="L48">
         <v>0.407281090129695</v>
       </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
       <c r="O48">
         <v>0.410010013883929</v>
       </c>
@@ -4269,6 +4413,12 @@
       <c r="L49">
         <v>0.403793944470449</v>
       </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
       <c r="O49">
         <v>0.291415600214873</v>
       </c>
@@ -4414,6 +4564,12 @@
       <c r="L51">
         <v>0.330754776712315</v>
       </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <v>0</v>
+      </c>
       <c r="O51">
         <v>0.350981323033059</v>
       </c>
@@ -4485,6 +4641,12 @@
       <c r="L52">
         <v>0.40868266233886</v>
       </c>
+      <c r="M52">
+        <v>0</v>
+      </c>
+      <c r="N52">
+        <v>0</v>
+      </c>
       <c r="O52">
         <v>0.152079389183164</v>
       </c>
@@ -4784,6 +4946,12 @@
       <c r="L56">
         <v>0.41525155702608</v>
       </c>
+      <c r="M56">
+        <v>0</v>
+      </c>
+      <c r="N56">
+        <v>0</v>
+      </c>
       <c r="O56">
         <v>0.28940231987449</v>
       </c>
@@ -5009,6 +5177,12 @@
       <c r="L59">
         <v>0.407281090129695</v>
       </c>
+      <c r="M59">
+        <v>0</v>
+      </c>
+      <c r="N59">
+        <v>0</v>
+      </c>
       <c r="O59">
         <v>0.392572211787595</v>
       </c>
@@ -5080,6 +5254,12 @@
       <c r="L60">
         <v>0.407281090129695</v>
       </c>
+      <c r="M60">
+        <v>0</v>
+      </c>
+      <c r="N60">
+        <v>0</v>
+      </c>
       <c r="O60">
         <v>0.411233924427668</v>
       </c>
@@ -5151,6 +5331,12 @@
       <c r="L61">
         <v>0.407281090129695</v>
       </c>
+      <c r="M61">
+        <v>0</v>
+      </c>
+      <c r="N61">
+        <v>0</v>
+      </c>
       <c r="O61">
         <v>0.41248804075057</v>
       </c>
@@ -5453,6 +5639,12 @@
       <c r="L65">
         <v>0.339605685126709</v>
       </c>
+      <c r="M65">
+        <v>0</v>
+      </c>
+      <c r="N65">
+        <v>0</v>
+      </c>
       <c r="O65">
         <v>0.280862452946929</v>
       </c>
@@ -5601,6 +5793,12 @@
       <c r="L67">
         <v>0.407281090129695</v>
       </c>
+      <c r="M67">
+        <v>0</v>
+      </c>
+      <c r="N67">
+        <v>0</v>
+      </c>
       <c r="O67">
         <v>0.384200350713085</v>
       </c>
@@ -5826,6 +6024,12 @@
       <c r="L70">
         <v>0.399510616283393</v>
       </c>
+      <c r="M70">
+        <v>0</v>
+      </c>
+      <c r="N70">
+        <v>0</v>
+      </c>
       <c r="O70">
         <v>0.33141835270053</v>
       </c>
@@ -5894,6 +6098,12 @@
       <c r="L71">
         <v>0.403793944470449</v>
       </c>
+      <c r="M71">
+        <v>0</v>
+      </c>
+      <c r="N71">
+        <v>0</v>
+      </c>
       <c r="O71">
         <v>0.341538423622197</v>
       </c>
@@ -6042,6 +6252,12 @@
       <c r="L73">
         <v>0.41525155702608</v>
       </c>
+      <c r="M73">
+        <v>0</v>
+      </c>
+      <c r="N73">
+        <v>0</v>
+      </c>
       <c r="O73">
         <v>0.319645417916082</v>
       </c>
@@ -6190,6 +6406,12 @@
       <c r="L75">
         <v>0.238984286945568</v>
       </c>
+      <c r="M75">
+        <v>0</v>
+      </c>
+      <c r="N75">
+        <v>0</v>
+      </c>
       <c r="O75">
         <v>0.333075438476568</v>
       </c>
@@ -6261,6 +6483,12 @@
       <c r="L76">
         <v>0.388003116567215</v>
       </c>
+      <c r="M76">
+        <v>0</v>
+      </c>
+      <c r="N76">
+        <v>0</v>
+      </c>
       <c r="O76">
         <v>0.31850421402075</v>
       </c>
@@ -6332,6 +6560,12 @@
       <c r="L77">
         <v>0.388003116567215</v>
       </c>
+      <c r="M77">
+        <v>0</v>
+      </c>
+      <c r="N77">
+        <v>0</v>
+      </c>
       <c r="O77">
         <v>0.353928144916681</v>
       </c>
@@ -6477,6 +6711,12 @@
       <c r="L79">
         <v>0.238984286945568</v>
       </c>
+      <c r="M79">
+        <v>0</v>
+      </c>
+      <c r="N79">
+        <v>0</v>
+      </c>
       <c r="O79">
         <v>0.402820441475505</v>
       </c>
@@ -6548,6 +6788,12 @@
       <c r="L80">
         <v>0.382118437118437</v>
       </c>
+      <c r="M80">
+        <v>0</v>
+      </c>
+      <c r="N80">
+        <v>0</v>
+      </c>
       <c r="O80">
         <v>0.271055299470911</v>
       </c>
@@ -6619,6 +6865,12 @@
       <c r="L81">
         <v>0.351464372989876</v>
       </c>
+      <c r="M81">
+        <v>0</v>
+      </c>
+      <c r="N81">
+        <v>0</v>
+      </c>
       <c r="O81">
         <v>0.315328319177625</v>
       </c>
@@ -6766,6 +7018,12 @@
       </c>
       <c r="L83">
         <v>0.351464372989876</v>
+      </c>
+      <c r="M83">
+        <v>0</v>
+      </c>
+      <c r="N83">
+        <v>0</v>
       </c>
       <c r="O83">
         <v>0.36105408341903</v>

</xml_diff>

<commit_message>
extrapolated and pc income
</commit_message>
<xml_diff>
--- a/inputs/all_data_compiled.xlsx
+++ b/inputs/all_data_compiled.xlsx
@@ -934,7 +934,7 @@
         <v>51</v>
       </c>
       <c r="B4">
-        <v>133.688</v>
+        <v>31.622466195801</v>
       </c>
       <c r="C4">
         <v>240135.244121424</v>
@@ -946,13 +946,13 @@
         <v>0.953416149068323</v>
       </c>
       <c r="F4">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G4">
-        <v>0.726025888549619</v>
+        <v>0.752295628751577</v>
       </c>
       <c r="H4">
-        <v>0.374005146310813</v>
+        <v>1.58115435053068</v>
       </c>
       <c r="I4">
         <v>0.693233188692644</v>
@@ -1011,7 +1011,7 @@
         <v>52</v>
       </c>
       <c r="B5">
-        <v>179.014</v>
+        <v>43.7266667519172</v>
       </c>
       <c r="C5">
         <v>661728.454375173</v>
@@ -1023,13 +1023,13 @@
         <v>0.821276595744681</v>
       </c>
       <c r="F5">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G5">
-        <v>0.972179989324558</v>
+        <v>1.04025347212522</v>
       </c>
       <c r="H5">
-        <v>0.279307763638598</v>
+        <v>1.14346698969017</v>
       </c>
       <c r="I5">
         <v>0.496879896983716</v>
@@ -1088,7 +1088,7 @@
         <v>53</v>
       </c>
       <c r="B6">
-        <v>126.492</v>
+        <v>30.8974355680757</v>
       </c>
       <c r="C6">
         <v>677779.68215436</v>
@@ -1100,13 +1100,13 @@
         <v>0.821276595744681</v>
       </c>
       <c r="F6">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G6">
-        <v>0.686946223254281</v>
+        <v>0.735047215279602</v>
       </c>
       <c r="H6">
-        <v>0.395281915061822</v>
+        <v>1.61825727866107</v>
       </c>
       <c r="I6">
         <v>0.475968914751725</v>
@@ -1165,7 +1165,7 @@
         <v>54</v>
       </c>
       <c r="B7">
-        <v>119.962</v>
+        <v>30.5156520200998</v>
       </c>
       <c r="C7">
         <v>554414.442422447</v>
@@ -1177,13 +1177,13 @@
         <v>0.823002754820937</v>
       </c>
       <c r="F7">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G7">
-        <v>0.651483436375661</v>
+        <v>0.725964618985777</v>
       </c>
       <c r="H7">
-        <v>0.416798652906754</v>
+        <v>1.63850341349634</v>
       </c>
       <c r="I7">
         <v>0.660083320158597</v>
@@ -1242,7 +1242,7 @@
         <v>55</v>
       </c>
       <c r="B8">
-        <v>158.629</v>
+        <v>33.7933125983381</v>
       </c>
       <c r="C8">
         <v>1264097.89496566</v>
@@ -1254,13 +1254,13 @@
         <v>0.8</v>
       </c>
       <c r="F8">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G8">
-        <v>0.861474183731804</v>
+        <v>0.803939869564668</v>
       </c>
       <c r="H8">
-        <v>0.315200877519243</v>
+        <v>1.47958267939849</v>
       </c>
       <c r="I8">
         <v>0.551314358767217</v>
@@ -1319,7 +1319,7 @@
         <v>56</v>
       </c>
       <c r="B9">
-        <v>124.667</v>
+        <v>31.7124988778928</v>
       </c>
       <c r="C9">
         <v>561980.471778846</v>
@@ -1331,13 +1331,13 @@
         <v>0.823002754820937</v>
       </c>
       <c r="F9">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G9">
-        <v>0.677035107472737</v>
+        <v>0.754437498166919</v>
       </c>
       <c r="H9">
-        <v>0.401068446341053</v>
+        <v>1.57666540856721</v>
       </c>
       <c r="I9">
         <v>0.437850462431834</v>
@@ -1396,7 +1396,7 @@
         <v>57</v>
       </c>
       <c r="B10">
-        <v>158.732</v>
+        <v>37.5463564732204</v>
       </c>
       <c r="C10">
         <v>116022.676390039</v>
@@ -1408,13 +1408,13 @@
         <v>0.953416149068323</v>
       </c>
       <c r="F10">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G10">
-        <v>0.86203355081427</v>
+        <v>0.893224446045983</v>
       </c>
       <c r="H10">
-        <v>0.314996346042386</v>
+        <v>1.33168713815579</v>
       </c>
       <c r="I10">
         <v>0.261279700917478</v>
@@ -1473,7 +1473,7 @@
         <v>58</v>
       </c>
       <c r="B11">
-        <v>175.235</v>
+        <v>40.970819598135</v>
       </c>
       <c r="C11">
         <v>207219.483546468</v>
@@ -1485,13 +1485,13 @@
         <v>1.0034516765286</v>
       </c>
       <c r="F11">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G11">
-        <v>0.951657191221295</v>
+        <v>0.974692116016529</v>
       </c>
       <c r="H11">
-        <v>0.28533112677262</v>
+        <v>1.22038076100084</v>
       </c>
       <c r="I11">
         <v>0.573358263824997</v>
@@ -1550,7 +1550,7 @@
         <v>59</v>
       </c>
       <c r="B12">
-        <v>134.8675</v>
+        <v>27.0121518182964</v>
       </c>
       <c r="C12">
         <v>404023.538097355</v>
@@ -1562,13 +1562,13 @@
         <v>0.66199649737303</v>
       </c>
       <c r="F12">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G12">
-        <v>0.732431456256102</v>
+        <v>0.642616664059449</v>
       </c>
       <c r="H12">
-        <v>0.370734239160658</v>
+        <v>1.85101876875033</v>
       </c>
       <c r="I12">
         <v>0.538168398955</v>
@@ -1627,7 +1627,7 @@
         <v>60</v>
       </c>
       <c r="B13">
-        <v>277.019</v>
+        <v>64.7684279639099</v>
       </c>
       <c r="C13">
         <v>716869.090163479</v>
@@ -1639,13 +1639,13 @@
         <v>1.0034516765286</v>
       </c>
       <c r="F13">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G13">
-        <v>1.5044204836644</v>
+        <v>1.54083508024529</v>
       </c>
       <c r="H13">
-        <v>0.180493034773788</v>
+        <v>0.771981065031574</v>
       </c>
       <c r="I13">
         <v>0.580481033452984</v>
@@ -1704,7 +1704,7 @@
         <v>61</v>
       </c>
       <c r="B14">
-        <v>316.686</v>
+        <v>68.1109768434638</v>
       </c>
       <c r="C14">
         <v>16631.5364730528</v>
@@ -1716,13 +1716,13 @@
         <v>0.895865237366003</v>
       </c>
       <c r="F14">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G14">
-        <v>1.719841979394</v>
+        <v>1.62035401768068</v>
       </c>
       <c r="H14">
-        <v>0.157885097541413</v>
+        <v>0.734096063765355</v>
       </c>
       <c r="I14">
         <v>0.391077905964043</v>
@@ -1778,7 +1778,7 @@
         <v>62</v>
       </c>
       <c r="B15">
-        <v>219.272</v>
+        <v>49.7660716793741</v>
       </c>
       <c r="C15">
         <v>2485002.05546474</v>
@@ -1790,13 +1790,13 @@
         <v>1.11720698254364</v>
       </c>
       <c r="F15">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G15">
-        <v>1.19081105734286</v>
+        <v>1.18393037256222</v>
       </c>
       <c r="H15">
-        <v>0.228027290306104</v>
+        <v>1.00470055828664</v>
       </c>
       <c r="I15">
         <v>0.601053603455341</v>
@@ -1855,7 +1855,7 @@
         <v>63</v>
       </c>
       <c r="B16">
-        <v>303.525</v>
+        <v>71.7955916169028</v>
       </c>
       <c r="C16">
         <v>754450.151792923</v>
@@ -1867,13 +1867,13 @@
         <v>0.953416149068323</v>
       </c>
       <c r="F16">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G16">
-        <v>1.64836790005104</v>
+        <v>1.70801067198868</v>
       </c>
       <c r="H16">
-        <v>0.164731076517585</v>
+        <v>0.696421589041249</v>
       </c>
       <c r="I16">
         <v>0.605775696080789</v>
@@ -1932,7 +1932,7 @@
         <v>64</v>
       </c>
       <c r="B17">
-        <v>237.761</v>
+        <v>49.8165407827101</v>
       </c>
       <c r="C17">
         <v>166437.019362635</v>
@@ -1944,13 +1944,13 @@
         <v>0.704046242774567</v>
       </c>
       <c r="F17">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G17">
-        <v>1.29122016401955</v>
+        <v>1.18513102799471</v>
       </c>
       <c r="H17">
-        <v>0.210295212419194</v>
+        <v>1.00368269683939</v>
       </c>
       <c r="I17">
         <v>0.611077177703641</v>
@@ -2009,7 +2009,7 @@
         <v>65</v>
       </c>
       <c r="B18">
-        <v>148.638</v>
+        <v>33.7692846625143</v>
       </c>
       <c r="C18">
         <v>1279708.23259846</v>
@@ -2021,13 +2021,13 @@
         <v>0.847161572052402</v>
       </c>
       <c r="F18">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G18">
-        <v>0.807215576732678</v>
+        <v>0.803368247130913</v>
       </c>
       <c r="H18">
-        <v>0.336387733957669</v>
+        <v>1.48063545022328</v>
       </c>
       <c r="I18">
         <v>0.566535444651524</v>
@@ -2086,7 +2086,7 @@
         <v>66</v>
       </c>
       <c r="B19">
-        <v>145.749</v>
+        <v>33.3653340831742</v>
       </c>
       <c r="C19">
         <v>1353046.84430757</v>
@@ -2098,13 +2098,13 @@
         <v>0.854588796185936</v>
       </c>
       <c r="F19">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G19">
-        <v>0.791526144681784</v>
+        <v>0.793758299153181</v>
       </c>
       <c r="H19">
-        <v>0.343055526967595</v>
+        <v>1.49856134739602</v>
       </c>
       <c r="I19">
         <v>0.496198567578322</v>
@@ -2163,7 +2163,7 @@
         <v>67</v>
       </c>
       <c r="B20">
-        <v>253.279</v>
+        <v>59.2178972065856</v>
       </c>
       <c r="C20">
         <v>3086241.84919508</v>
@@ -2175,13 +2175,13 @@
         <v>1.0034516765286</v>
       </c>
       <c r="F20">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G20">
-        <v>1.37549451727873</v>
+        <v>1.40878845237852</v>
       </c>
       <c r="H20">
-        <v>0.197410760465731</v>
+        <v>0.84433933588644</v>
       </c>
       <c r="I20">
         <v>0.601417335117009</v>
@@ -2240,7 +2240,7 @@
         <v>68</v>
       </c>
       <c r="B21">
-        <v>179.424</v>
+        <v>38.5894668825324</v>
       </c>
       <c r="C21">
         <v>1153021.19591091</v>
@@ -2252,13 +2252,13 @@
         <v>0.895865237366003</v>
       </c>
       <c r="F21">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G21">
-        <v>0.974406596157671</v>
+        <v>0.918039948934714</v>
       </c>
       <c r="H21">
-        <v>0.278669520242554</v>
+        <v>1.2956903538523</v>
       </c>
       <c r="I21">
         <v>0.605970067589554</v>
@@ -2317,7 +2317,7 @@
         <v>69</v>
       </c>
       <c r="B22">
-        <v>149.238</v>
+        <v>31.7927137254272</v>
       </c>
       <c r="C22">
         <v>558647.498120183</v>
@@ -2329,13 +2329,13 @@
         <v>0.8</v>
       </c>
       <c r="F22">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G22">
-        <v>0.810474025756747</v>
+        <v>0.756345802180509</v>
       </c>
       <c r="H22">
-        <v>0.335035312721961</v>
+        <v>1.57268739094804</v>
       </c>
       <c r="I22">
         <v>0.625601602025372</v>
@@ -2394,7 +2394,7 @@
         <v>70</v>
       </c>
       <c r="B23">
-        <v>152.074</v>
+        <v>32.3968771162881</v>
       </c>
       <c r="C23">
         <v>1881962.89125995</v>
@@ -2406,13 +2406,13 @@
         <v>0.8</v>
       </c>
       <c r="F23">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G23">
-        <v>0.825875628143848</v>
+        <v>0.770718794950339</v>
       </c>
       <c r="H23">
-        <v>0.328787300919289</v>
+        <v>1.54335863362773</v>
       </c>
       <c r="I23">
         <v>0.61358913909323</v>
@@ -2471,7 +2471,7 @@
         <v>71</v>
       </c>
       <c r="B24">
-        <v>156.261</v>
+        <v>35.7717752380523</v>
       </c>
       <c r="C24">
         <v>85865.384952272</v>
@@ -2483,13 +2483,13 @@
         <v>0.854588796185936</v>
       </c>
       <c r="F24">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G24">
-        <v>0.848614171583478</v>
+        <v>0.851007317950554</v>
       </c>
       <c r="H24">
-        <v>0.31997747358586</v>
+        <v>1.3977500324561</v>
       </c>
       <c r="I24">
         <v>0.704419697775541</v>
@@ -2548,7 +2548,7 @@
         <v>72</v>
       </c>
       <c r="B25">
-        <v>177.386</v>
+        <v>45.123034371196</v>
       </c>
       <c r="C25">
         <v>733558.367597268</v>
@@ -2560,13 +2560,13 @@
         <v>0.823002754820937</v>
       </c>
       <c r="F25">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G25">
-        <v>0.963338730972583</v>
+        <v>1.07347293229032</v>
       </c>
       <c r="H25">
-        <v>0.281871173598818</v>
+        <v>1.10808150863004</v>
       </c>
       <c r="I25">
         <v>0.593455555845053</v>
@@ -2625,7 +2625,7 @@
         <v>73</v>
       </c>
       <c r="B26">
-        <v>241.147</v>
+        <v>51.37242214949</v>
       </c>
       <c r="C26">
         <v>253003.132887467</v>
@@ -2637,13 +2637,13 @@
         <v>0.8</v>
       </c>
       <c r="F26">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G26">
-        <v>1.30960867801205</v>
+        <v>1.22214530587667</v>
       </c>
       <c r="H26">
-        <v>0.207342409401734</v>
+        <v>0.973284846381268</v>
       </c>
       <c r="I26">
         <v>0.623269968447109</v>
@@ -2702,7 +2702,7 @@
         <v>74</v>
       </c>
       <c r="B27">
-        <v>282.606</v>
+        <v>64.1403847870279</v>
       </c>
       <c r="C27">
         <v>3350889.3025638</v>
@@ -2714,13 +2714,13 @@
         <v>1.11720698254364</v>
       </c>
       <c r="F27">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G27">
-        <v>1.53476207482686</v>
+        <v>1.52589398951219</v>
       </c>
       <c r="H27">
-        <v>0.176924764513138</v>
+        <v>0.779540069271806</v>
       </c>
       <c r="I27">
         <v>0.656626150696792</v>
@@ -2779,7 +2779,7 @@
         <v>75</v>
       </c>
       <c r="B28">
-        <v>207.478</v>
+        <v>47.137230339544</v>
       </c>
       <c r="C28">
         <v>4351713.3885828</v>
@@ -2791,13 +2791,13 @@
         <v>0.847161572052402</v>
       </c>
       <c r="F28">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G28">
-        <v>1.1267608110264</v>
+        <v>1.12139047335289</v>
       </c>
       <c r="H28">
-        <v>0.240989406105708</v>
+        <v>1.0607326658744</v>
       </c>
       <c r="I28">
         <v>0.510060947320871</v>
@@ -2856,7 +2856,7 @@
         <v>76</v>
       </c>
       <c r="B29">
-        <v>137.747</v>
+        <v>32.5146016591531</v>
       </c>
       <c r="C29">
         <v>710843.272307041</v>
@@ -2868,13 +2868,13 @@
         <v>0.861990950226244</v>
       </c>
       <c r="F29">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G29">
-        <v>0.748069296197447</v>
+        <v>0.773519451244686</v>
       </c>
       <c r="H29">
-        <v>0.362984311818043</v>
+        <v>1.53777064606679</v>
       </c>
       <c r="I29">
         <v>0.449828573348919</v>
@@ -2933,7 +2933,7 @@
         <v>77</v>
       </c>
       <c r="B30">
-        <v>156.283</v>
+        <v>36.8899467218699</v>
       </c>
       <c r="C30">
         <v>992308.737024673</v>
@@ -2945,13 +2945,13 @@
         <v>0.861990950226244</v>
       </c>
       <c r="F30">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G30">
-        <v>0.848733648047693</v>
+        <v>0.877608517055713</v>
       </c>
       <c r="H30">
-        <v>0.319932430270727</v>
+        <v>1.35538281952459</v>
       </c>
       <c r="I30">
         <v>0.539234654715103</v>
@@ -3010,7 +3010,7 @@
         <v>78</v>
       </c>
       <c r="B31">
-        <v>190.398</v>
+        <v>44.9426493985308</v>
       </c>
       <c r="C31">
         <v>2410527.96165012</v>
@@ -3022,13 +3022,13 @@
         <v>0.861990950226244</v>
       </c>
       <c r="F31">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G31">
-        <v>1.0340036288079</v>
+        <v>1.06918159000258</v>
       </c>
       <c r="H31">
-        <v>0.262607800502106</v>
+        <v>1.11252898236201</v>
       </c>
       <c r="I31">
         <v>0.568224630141931</v>
@@ -3087,7 +3087,7 @@
         <v>79</v>
       </c>
       <c r="B32">
-        <v>97.289</v>
+        <v>22.9646604341099</v>
       </c>
       <c r="C32">
         <v>533220.801373149</v>
@@ -3099,13 +3099,13 @@
         <v>0.861990950226244</v>
       </c>
       <c r="F32">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G32">
-        <v>0.528352078504457</v>
+        <v>0.546327207795047</v>
       </c>
       <c r="H32">
-        <v>0.513932715928831</v>
+        <v>2.17725840725839</v>
       </c>
       <c r="I32">
         <v>0.505140012725683</v>
@@ -3173,7 +3173,7 @@
         <v>0.821276595744681</v>
       </c>
       <c r="F33">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="I33">
         <v>0.931293981832552</v>
@@ -3226,7 +3226,7 @@
         <v>81</v>
       </c>
       <c r="B34">
-        <v>130.115</v>
+        <v>27.2621632813721</v>
       </c>
       <c r="C34">
         <v>440354.934932028</v>
@@ -3238,13 +3238,13 @@
         <v>0.704046242774567</v>
       </c>
       <c r="F34">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G34">
-        <v>0.706621824611286</v>
+        <v>0.64856441429642</v>
       </c>
       <c r="H34">
-        <v>0.384275448641586</v>
+        <v>1.83404374348254</v>
       </c>
       <c r="I34">
         <v>0.5052488202008</v>
@@ -3303,7 +3303,7 @@
         <v>82</v>
       </c>
       <c r="B35">
-        <v>162.895</v>
+        <v>41.4368478002547</v>
       </c>
       <c r="C35">
         <v>167618.61939646</v>
@@ -3315,13 +3315,13 @@
         <v>0.823002754820937</v>
       </c>
       <c r="F35">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G35">
-        <v>0.884641756292937</v>
+        <v>0.985778885061004</v>
       </c>
       <c r="H35">
-        <v>0.306946192332484</v>
+        <v>1.20665549273979</v>
       </c>
       <c r="I35">
         <v>0.437850462431834</v>
@@ -3380,7 +3380,7 @@
         <v>83</v>
       </c>
       <c r="B36">
-        <v>149.062</v>
+        <v>35.2590214236019</v>
       </c>
       <c r="C36">
         <v>197584.190285786</v>
@@ -3392,13 +3392,13 @@
         <v>0.953416149068323</v>
       </c>
       <c r="F36">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G36">
-        <v>0.80951821404302</v>
+        <v>0.838808950788161</v>
       </c>
       <c r="H36">
-        <v>0.33543089452711</v>
+        <v>1.41807679229948</v>
       </c>
       <c r="I36">
         <v>0.499190243762243</v>
@@ -3457,7 +3457,7 @@
         <v>84</v>
       </c>
       <c r="B37">
-        <v>192.382</v>
+        <v>42.1019856131476</v>
       </c>
       <c r="C37">
         <v>579429.044110523</v>
@@ -3469,13 +3469,13 @@
         <v>0.886567164179105</v>
       </c>
       <c r="F37">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G37">
-        <v>1.04477823358082</v>
+        <v>1.00160245385094</v>
       </c>
       <c r="H37">
-        <v>0.259899574804296</v>
+        <v>1.18759244420021</v>
       </c>
       <c r="I37">
         <v>0.614787928154712</v>
@@ -3534,7 +3534,7 @@
         <v>85</v>
       </c>
       <c r="B38">
-        <v>175.91</v>
+        <v>38.4971582019565</v>
       </c>
       <c r="C38">
         <v>672277.192943119</v>
@@ -3546,13 +3546,13 @@
         <v>0.886567164179105</v>
       </c>
       <c r="F38">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G38">
-        <v>0.955322946373372</v>
+        <v>0.91584393371999</v>
       </c>
       <c r="H38">
-        <v>0.284236257176965</v>
+        <v>1.2987971667337</v>
       </c>
       <c r="I38">
         <v>0.643920540702937</v>
@@ -3611,7 +3611,7 @@
         <v>86</v>
       </c>
       <c r="B39">
-        <v>187.023</v>
+        <v>47.5744718140338</v>
       </c>
       <c r="C39">
         <v>2296674.28518162</v>
@@ -3623,13 +3623,13 @@
         <v>0.823002754820937</v>
       </c>
       <c r="F39">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G39">
-        <v>1.01567485304751</v>
+        <v>1.13179240873424</v>
       </c>
       <c r="H39">
-        <v>0.267346796918026</v>
+        <v>1.0509838174441</v>
       </c>
       <c r="I39">
         <v>0.54518290933124</v>
@@ -3688,7 +3688,7 @@
         <v>87</v>
       </c>
       <c r="B40">
-        <v>169.871</v>
+        <v>36.5348633895279</v>
       </c>
       <c r="C40">
         <v>1533715.59215201</v>
@@ -3700,13 +3700,13 @@
         <v>0.895865237366003</v>
       </c>
       <c r="F40">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G40">
-        <v>0.922526656946115</v>
+        <v>0.869161116492157</v>
       </c>
       <c r="H40">
-        <v>0.294340999935245</v>
+        <v>1.36855582206259</v>
       </c>
       <c r="I40">
         <v>0.600693080642694</v>
@@ -3765,7 +3765,7 @@
         <v>88</v>
       </c>
       <c r="B41">
-        <v>170.385</v>
+        <v>40.3027489585569</v>
       </c>
       <c r="C41">
         <v>207635.165378523</v>
@@ -3777,13 +3777,13 @@
         <v>0.953416149068323</v>
       </c>
       <c r="F41">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G41">
-        <v>0.925318061610068</v>
+        <v>0.958798775543336</v>
       </c>
       <c r="H41">
-        <v>0.293453062182704</v>
+        <v>1.24061016412093</v>
       </c>
       <c r="I41">
         <v>0.607822777429657</v>
@@ -3842,7 +3842,7 @@
         <v>89</v>
       </c>
       <c r="B42">
-        <v>206.399</v>
+        <v>45.1695466757184</v>
       </c>
       <c r="C42">
         <v>759942.515079343</v>
@@ -3854,13 +3854,13 @@
         <v>0.886567164179105</v>
       </c>
       <c r="F42">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G42">
-        <v>1.12090103353145</v>
+        <v>1.07457945583464</v>
       </c>
       <c r="H42">
-        <v>0.242249235703661</v>
+        <v>1.10694048711537</v>
       </c>
       <c r="I42">
         <v>0.581058264319275</v>
@@ -3919,7 +3919,7 @@
         <v>90</v>
       </c>
       <c r="B43">
-        <v>249.092</v>
+        <v>56.534032283003</v>
       </c>
       <c r="C43">
         <v>2838393.48641403</v>
@@ -3931,13 +3931,13 @@
         <v>1.11720698254364</v>
       </c>
       <c r="F43">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G43">
-        <v>1.3527559738391</v>
+        <v>1.34493954705693</v>
       </c>
       <c r="H43">
-        <v>0.20072904790198</v>
+        <v>0.884423027703129</v>
       </c>
       <c r="I43">
         <v>0.592091447554131</v>
@@ -3996,7 +3996,7 @@
         <v>91</v>
       </c>
       <c r="B44">
-        <v>164.672</v>
+        <v>37.6972486544982</v>
       </c>
       <c r="C44">
         <v>969716.979767905</v>
@@ -4008,13 +4008,13 @@
         <v>0.854588796185936</v>
       </c>
       <c r="F44">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G44">
-        <v>0.894292196152555</v>
+        <v>0.896814157477256</v>
       </c>
       <c r="H44">
-        <v>0.303633890400311</v>
+        <v>1.32635674444728</v>
       </c>
       <c r="I44">
         <v>0.556690327994871</v>
@@ -4073,7 +4073,7 @@
         <v>92</v>
       </c>
       <c r="B45">
-        <v>131.981</v>
+        <v>26.4340245732336</v>
       </c>
       <c r="C45">
         <v>962426.556333156</v>
@@ -4085,13 +4085,13 @@
         <v>0.66199649737303</v>
       </c>
       <c r="F45">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G45">
-        <v>0.716755601076142</v>
+        <v>0.628863068858177</v>
       </c>
       <c r="H45">
-        <v>0.378842409134648</v>
+        <v>1.89150160852271</v>
       </c>
       <c r="I45">
         <v>0.39129314485286</v>
@@ -4150,7 +4150,7 @@
         <v>93</v>
       </c>
       <c r="B46">
-        <v>178.397</v>
+        <v>37.378381761572</v>
       </c>
       <c r="C46">
         <v>1831350.58211375</v>
@@ -4162,13 +4162,13 @@
         <v>0.704046242774567</v>
       </c>
       <c r="F46">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G46">
-        <v>0.968829217578139</v>
+        <v>0.889228342752476</v>
       </c>
       <c r="H46">
-        <v>0.280273771419923</v>
+        <v>1.33767160705186</v>
       </c>
       <c r="I46">
         <v>0.533733685257792</v>
@@ -4227,7 +4227,7 @@
         <v>94</v>
       </c>
       <c r="B47">
-        <v>140.218</v>
+        <v>28.0837852237039</v>
       </c>
       <c r="C47">
         <v>1274192.94879532</v>
@@ -4239,13 +4239,13 @@
         <v>0.66199649737303</v>
       </c>
       <c r="F47">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G47">
-        <v>0.761488675428239</v>
+        <v>0.668110726461808</v>
       </c>
       <c r="H47">
-        <v>0.356587599309646</v>
+        <v>1.78038678197118</v>
       </c>
       <c r="I47">
         <v>0.39129314485286</v>
@@ -4304,7 +4304,7 @@
         <v>95</v>
       </c>
       <c r="B48">
-        <v>151.717</v>
+        <v>38.4011620078997</v>
       </c>
       <c r="C48">
         <v>229974.564772054</v>
@@ -4316,13 +4316,13 @@
         <v>0.791525423728814</v>
       </c>
       <c r="F48">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G48">
-        <v>0.823936850974527</v>
+        <v>0.913560192890968</v>
       </c>
       <c r="H48">
-        <v>0.329560958890566</v>
+        <v>1.30204393267355</v>
       </c>
       <c r="I48">
         <v>0.731612824879396</v>
@@ -4381,7 +4381,7 @@
         <v>96</v>
       </c>
       <c r="B49">
-        <v>126.563</v>
+        <v>26.9621760358035</v>
       </c>
       <c r="C49">
         <v>862659.413376048</v>
@@ -4393,13 +4393,13 @@
         <v>0.8</v>
       </c>
       <c r="F49">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G49">
-        <v>0.687331806388796</v>
+        <v>0.64142774468548</v>
       </c>
       <c r="H49">
-        <v>0.395060167663535</v>
+        <v>1.85444972741088</v>
       </c>
       <c r="I49">
         <v>0.55283948979472</v>
@@ -4458,7 +4458,7 @@
         <v>97</v>
       </c>
       <c r="B50">
-        <v>116.277</v>
+        <v>26.618508196895</v>
       </c>
       <c r="C50">
         <v>585373.492033969</v>
@@ -4470,13 +4470,13 @@
         <v>0.854588796185936</v>
       </c>
       <c r="F50">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G50">
-        <v>0.631471128619502</v>
+        <v>0.633251917684749</v>
       </c>
       <c r="H50">
-        <v>0.430007654136244</v>
+        <v>1.87839226864834</v>
       </c>
       <c r="I50">
         <v>0.647841827821625</v>
@@ -4532,7 +4532,7 @@
         <v>98</v>
       </c>
       <c r="B51">
-        <v>205.538</v>
+        <v>47.052425998034</v>
       </c>
       <c r="C51">
         <v>1482282.67149162</v>
@@ -4544,13 +4544,13 @@
         <v>0.854588796185936</v>
       </c>
       <c r="F51">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G51">
-        <v>1.11622515918191</v>
+        <v>1.1193729856901</v>
       </c>
       <c r="H51">
-        <v>0.243264019305433</v>
+        <v>1.06264446390265</v>
       </c>
       <c r="I51">
         <v>0.543458672242409</v>
@@ -4609,7 +4609,7 @@
         <v>99</v>
       </c>
       <c r="B52">
-        <v>122.076</v>
+        <v>28.8757718218434</v>
       </c>
       <c r="C52">
         <v>157051.141451002</v>
@@ -4621,13 +4621,13 @@
         <v>0.953416149068323</v>
       </c>
       <c r="F52">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G52">
-        <v>0.662964038437132</v>
+        <v>0.686952016452318</v>
       </c>
       <c r="H52">
-        <v>0.409580916805924</v>
+        <v>1.73155544753879</v>
       </c>
       <c r="I52">
         <v>0.637626431996089</v>
@@ -4686,7 +4686,7 @@
         <v>100</v>
       </c>
       <c r="B53">
-        <v>145.959</v>
+        <v>37.1287078675059</v>
       </c>
       <c r="C53">
         <v>2981577.20469059</v>
@@ -4698,13 +4698,13 @@
         <v>0.823002754820937</v>
       </c>
       <c r="F53">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G53">
-        <v>0.792666601840208</v>
+        <v>0.883288623251905</v>
       </c>
       <c r="H53">
-        <v>0.342561952329079</v>
+        <v>1.34666684815495</v>
       </c>
       <c r="I53">
         <v>0.584921770775726</v>
@@ -4763,7 +4763,7 @@
         <v>101</v>
       </c>
       <c r="B54">
-        <v>146.286</v>
+        <v>33.2349303417737</v>
       </c>
       <c r="C54">
         <v>1320494.31934513</v>
@@ -4775,13 +4775,13 @@
         <v>0.847161572052402</v>
       </c>
       <c r="F54">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G54">
-        <v>0.794442456558326</v>
+        <v>0.790656005865207</v>
       </c>
       <c r="H54">
-        <v>0.341796207429282</v>
+        <v>1.50444124557571</v>
       </c>
       <c r="I54">
         <v>0.559499847441382</v>
@@ -4837,7 +4837,7 @@
         <v>102</v>
       </c>
       <c r="B55">
-        <v>136.889</v>
+        <v>30.1683937042615</v>
       </c>
       <c r="C55">
         <v>1288466.35114615</v>
@@ -4849,13 +4849,13 @@
         <v>0.881398252184769</v>
       </c>
       <c r="F55">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G55">
-        <v>0.743409714093028</v>
+        <v>0.717703374861577</v>
       </c>
       <c r="H55">
-        <v>0.365259443782919</v>
+        <v>1.65736367968896</v>
       </c>
       <c r="I55">
         <v>0.473517553705807</v>
@@ -4914,7 +4914,7 @@
         <v>103</v>
       </c>
       <c r="B56">
-        <v>137.606</v>
+        <v>28.8317045728509</v>
       </c>
       <c r="C56">
         <v>608478.055899388</v>
@@ -4926,13 +4926,13 @@
         <v>0.704046242774567</v>
       </c>
       <c r="F56">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G56">
-        <v>0.747303560676791</v>
+        <v>0.685903660559299</v>
       </c>
       <c r="H56">
-        <v>0.36335624900077</v>
+        <v>1.73420200923819</v>
       </c>
       <c r="I56">
         <v>0.472971887518146</v>
@@ -4991,7 +4991,7 @@
         <v>104</v>
       </c>
       <c r="B57">
-        <v>169.592</v>
+        <v>39.651457969509</v>
       </c>
       <c r="C57">
         <v>2020505.5211558</v>
@@ -5003,13 +5003,13 @@
         <v>1.0034516765286</v>
       </c>
       <c r="F57">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G57">
-        <v>0.921011478149923</v>
+        <v>0.943304621448199</v>
       </c>
       <c r="H57">
-        <v>0.294825227605076</v>
+        <v>1.26098768016169</v>
       </c>
       <c r="I57">
         <v>0.66171307823978</v>
@@ -5068,7 +5068,7 @@
         <v>105</v>
       </c>
       <c r="B58">
-        <v>214.169</v>
+        <v>46.0622187263971</v>
       </c>
       <c r="C58">
         <v>433165.204738251</v>
@@ -5080,13 +5080,13 @@
         <v>0.895865237366003</v>
       </c>
       <c r="F58">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G58">
-        <v>1.16309794839315</v>
+        <v>1.09581604369203</v>
       </c>
       <c r="H58">
-        <v>0.233460491481027</v>
+        <v>1.08548831086476</v>
       </c>
       <c r="I58">
         <v>0.594974157700887</v>
@@ -5145,7 +5145,7 @@
         <v>106</v>
       </c>
       <c r="B59">
-        <v>166.109</v>
+        <v>42.0439279709605</v>
       </c>
       <c r="C59">
         <v>469105.617677937</v>
@@ -5157,13 +5157,13 @@
         <v>0.791525423728814</v>
       </c>
       <c r="F59">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G59">
-        <v>0.902096181565201</v>
+        <v>1.0002212677612</v>
       </c>
       <c r="H59">
-        <v>0.301007169990789</v>
+        <v>1.18923236750226</v>
       </c>
       <c r="I59">
         <v>0.686160742512875</v>
@@ -5222,7 +5222,7 @@
         <v>107</v>
       </c>
       <c r="B60">
-        <v>142.899</v>
+        <v>36.1692338351461</v>
       </c>
       <c r="C60">
         <v>808182.428935386</v>
@@ -5234,13 +5234,13 @@
         <v>0.791525423728814</v>
       </c>
       <c r="F60">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G60">
-        <v>0.776048511817455</v>
+        <v>0.860462822254108</v>
       </c>
       <c r="H60">
-        <v>0.349897480038349</v>
+        <v>1.38239035496003</v>
       </c>
       <c r="I60">
         <v>0.628316940328756</v>
@@ -5299,7 +5299,7 @@
         <v>108</v>
       </c>
       <c r="B61">
-        <v>132.64</v>
+        <v>33.5725734672305</v>
       </c>
       <c r="C61">
         <v>1050521.91485667</v>
@@ -5311,13 +5311,13 @@
         <v>0.791525423728814</v>
       </c>
       <c r="F61">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G61">
-        <v>0.720334464254244</v>
+        <v>0.79868850547439</v>
       </c>
       <c r="H61">
-        <v>0.376960193003619</v>
+        <v>1.48931091174181</v>
       </c>
       <c r="I61">
         <v>0.593796075486402</v>
@@ -5376,7 +5376,7 @@
         <v>109</v>
       </c>
       <c r="B62">
-        <v>235.621</v>
+        <v>55.0893684739474</v>
       </c>
       <c r="C62">
         <v>2444446.17134412</v>
@@ -5388,13 +5388,13 @@
         <v>1.0034516765286</v>
       </c>
       <c r="F62">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G62">
-        <v>1.27959836250037</v>
+        <v>1.31057112487762</v>
       </c>
       <c r="H62">
-        <v>0.212205193934327</v>
+        <v>0.907616140556154</v>
       </c>
       <c r="I62">
         <v>0.58379321753871</v>
@@ -5453,7 +5453,7 @@
         <v>110</v>
       </c>
       <c r="B63">
-        <v>182.388</v>
+        <v>39.914841055872</v>
       </c>
       <c r="C63">
         <v>2854701.4824351</v>
@@ -5465,13 +5465,13 @@
         <v>0.886567164179105</v>
       </c>
       <c r="F63">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G63">
-        <v>0.990503334336574</v>
+        <v>0.949570481401407</v>
       </c>
       <c r="H63">
-        <v>0.274140842599294</v>
+        <v>1.25266689475253</v>
       </c>
       <c r="I63">
         <v>0.635505299806107</v>
@@ -5530,7 +5530,7 @@
         <v>111</v>
       </c>
       <c r="B64">
-        <v>179.092</v>
+        <v>40.6468008190852</v>
       </c>
       <c r="C64">
         <v>2055103.11595472</v>
@@ -5542,13 +5542,13 @@
         <v>1.11720698254364</v>
       </c>
       <c r="F64">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G64">
-        <v>0.972603587697687</v>
+        <v>0.966983738383891</v>
       </c>
       <c r="H64">
-        <v>0.279186116632792</v>
+        <v>1.2301091104942</v>
       </c>
       <c r="I64">
         <v>0.589964760829172</v>
@@ -5607,7 +5607,7 @@
         <v>112</v>
       </c>
       <c r="B65">
-        <v>199.391</v>
+        <v>42.883852724134</v>
       </c>
       <c r="C65">
         <v>183040.964516342</v>
@@ -5619,13 +5619,13 @@
         <v>0.895865237366003</v>
       </c>
       <c r="F65">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G65">
-        <v>1.08284234893032</v>
+        <v>1.02020300215156</v>
       </c>
       <c r="H65">
-        <v>0.250763575086137</v>
+        <v>1.16594001760157</v>
       </c>
       <c r="I65">
         <v>0.506628945908215</v>
@@ -5684,7 +5684,7 @@
         <v>113</v>
       </c>
       <c r="B66">
-        <v>294.404</v>
+        <v>66.8180641700465</v>
       </c>
       <c r="C66">
         <v>2678553.46348061</v>
@@ -5696,13 +5696,13 @@
         <v>1.11720698254364</v>
       </c>
       <c r="F66">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G66">
-        <v>1.59883404413681</v>
+        <v>1.58959574137969</v>
       </c>
       <c r="H66">
-        <v>0.169834648985747</v>
+        <v>0.748300637276083</v>
       </c>
       <c r="I66">
         <v>0.548077987002169</v>
@@ -5761,7 +5761,7 @@
         <v>114</v>
       </c>
       <c r="B67">
-        <v>121.06</v>
+        <v>30.6415541612103</v>
       </c>
       <c r="C67">
         <v>288015.178598222</v>
@@ -5773,13 +5773,13 @@
         <v>0.791525423728814</v>
       </c>
       <c r="F67">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G67">
-        <v>0.657446398089708</v>
+        <v>0.728959819607431</v>
       </c>
       <c r="H67">
-        <v>0.413018338014208</v>
+        <v>1.63177101712732</v>
       </c>
       <c r="I67">
         <v>0.523882135324561</v>
@@ -5838,7 +5838,7 @@
         <v>115</v>
       </c>
       <c r="B68">
-        <v>134.968</v>
+        <v>28.278981314685</v>
       </c>
       <c r="C68">
         <v>753363.084895201</v>
@@ -5850,13 +5850,13 @@
         <v>0.704046242774567</v>
       </c>
       <c r="F68">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G68">
-        <v>0.732977246467633</v>
+        <v>0.672754423923139</v>
       </c>
       <c r="H68">
-        <v>0.370458182680339</v>
+        <v>1.76809763561163</v>
       </c>
       <c r="I68">
         <v>0.59513193838165</v>
@@ -5915,7 +5915,7 @@
         <v>116</v>
       </c>
       <c r="B69">
-        <v>107.685</v>
+        <v>23.7322463897274</v>
       </c>
       <c r="C69">
         <v>518718.742502788</v>
@@ -5927,13 +5927,13 @@
         <v>0.881398252184769</v>
       </c>
       <c r="F69">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G69">
-        <v>0.58481013859483</v>
+        <v>0.564588008692948</v>
       </c>
       <c r="H69">
-        <v>0.464317221525746</v>
+        <v>2.10683806239441</v>
       </c>
       <c r="I69">
         <v>0.492333585156966</v>
@@ -5992,7 +5992,7 @@
         <v>117</v>
       </c>
       <c r="B70">
-        <v>106.487</v>
+        <v>24.1929373098209</v>
       </c>
       <c r="C70">
         <v>93087.5521866449</v>
@@ -6004,13 +6004,13 @@
         <v>0.847161572052402</v>
       </c>
       <c r="F70">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G70">
-        <v>0.578304102043439</v>
+        <v>0.575547804277705</v>
       </c>
       <c r="H70">
-        <v>0.469540882924676</v>
+        <v>2.066718867564</v>
       </c>
       <c r="I70">
         <v>0.566535444651524</v>
@@ -6066,7 +6066,7 @@
         <v>118</v>
       </c>
       <c r="B71">
-        <v>142.671</v>
+        <v>30.3937218397487</v>
       </c>
       <c r="C71">
         <v>760233.378851882</v>
@@ -6078,13 +6078,13 @@
         <v>0.8</v>
       </c>
       <c r="F71">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G71">
-        <v>0.774810301188309</v>
+        <v>0.723063910953613</v>
       </c>
       <c r="H71">
-        <v>0.350456645008446</v>
+        <v>1.64507658073683</v>
       </c>
       <c r="I71">
         <v>0.603894799228239</v>
@@ -6143,7 +6143,7 @@
         <v>119</v>
       </c>
       <c r="B72">
-        <v>191.36</v>
+        <v>42.1730293832775</v>
       </c>
       <c r="C72">
         <v>1424914.17073343</v>
@@ -6155,13 +6155,13 @@
         <v>0.881398252184769</v>
       </c>
       <c r="F72">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G72">
-        <v>1.03922800874316</v>
+        <v>1.00329257875732</v>
       </c>
       <c r="H72">
-        <v>0.26128762541806</v>
+        <v>1.18559185173987</v>
       </c>
       <c r="I72">
         <v>0.554653565394186</v>
@@ -6220,7 +6220,7 @@
         <v>120</v>
       </c>
       <c r="B73">
-        <v>141.614</v>
+        <v>29.6714751637262</v>
       </c>
       <c r="C73">
         <v>407424.6404592</v>
@@ -6232,13 +6232,13 @@
         <v>0.704046242774567</v>
       </c>
       <c r="F73">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G73">
-        <v>0.769070000157574</v>
+        <v>0.705881727442441</v>
       </c>
       <c r="H73">
-        <v>0.35307243634104</v>
+        <v>1.68512012712889</v>
       </c>
       <c r="I73">
         <v>0.612978966276617</v>
@@ -6297,7 +6297,7 @@
         <v>121</v>
       </c>
       <c r="B74">
-        <v>113.736</v>
+        <v>25.0658009507549</v>
       </c>
       <c r="C74">
         <v>784135.419521753</v>
@@ -6309,13 +6309,13 @@
         <v>0.881398252184769</v>
       </c>
       <c r="F74">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G74">
-        <v>0.617671597002569</v>
+        <v>0.596313151847528</v>
       </c>
       <c r="H74">
-        <v>0.439614545966097</v>
+        <v>1.99474974281619</v>
       </c>
       <c r="I74">
         <v>0.595014685694195</v>
@@ -6374,7 +6374,7 @@
         <v>122</v>
       </c>
       <c r="B75">
-        <v>109.666</v>
+        <v>21.9646292939759</v>
       </c>
       <c r="C75">
         <v>739823.241271958</v>
@@ -6386,13 +6386,13 @@
         <v>0.66199649737303</v>
       </c>
       <c r="F75">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G75">
-        <v>0.595568451122632</v>
+        <v>0.522536556848341</v>
       </c>
       <c r="H75">
-        <v>0.455929823281601</v>
+        <v>2.27638715549428</v>
       </c>
       <c r="I75">
         <v>0.62421925110961</v>
@@ -6451,7 +6451,7 @@
         <v>123</v>
       </c>
       <c r="B76">
-        <v>139.481</v>
+        <v>34.0701800151059</v>
       </c>
       <c r="C76">
         <v>457632.980184378</v>
@@ -6463,13 +6463,13 @@
         <v>0.821276595744681</v>
       </c>
       <c r="F76">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G76">
-        <v>0.757486213877007</v>
+        <v>0.810526520526311</v>
       </c>
       <c r="H76">
-        <v>0.358471763179214</v>
+        <v>1.46755902017046</v>
       </c>
       <c r="I76">
         <v>0.561360301890219</v>
@@ -6528,7 +6528,7 @@
         <v>124</v>
       </c>
       <c r="B77">
-        <v>141.879</v>
+        <v>34.6559249672945</v>
       </c>
       <c r="C77">
         <v>573919.951416108</v>
@@ -6540,13 +6540,13 @@
         <v>0.821276595744681</v>
       </c>
       <c r="F77">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G77">
-        <v>0.770509148476537</v>
+        <v>0.824461340295471</v>
       </c>
       <c r="H77">
-        <v>0.352412971616659</v>
+        <v>1.44275473954846</v>
       </c>
       <c r="I77">
         <v>0.57325688846045</v>
@@ -6602,7 +6602,7 @@
         <v>125</v>
       </c>
       <c r="B78">
-        <v>190.392</v>
+        <v>44.5146020197342</v>
       </c>
       <c r="C78">
         <v>1318604.09835682</v>
@@ -6614,13 +6614,13 @@
         <v>1.0034516765286</v>
       </c>
       <c r="F78">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G78">
-        <v>1.03397104431766</v>
+        <v>1.05899838133146</v>
       </c>
       <c r="H78">
-        <v>0.262616076305727</v>
+        <v>1.12322693523878</v>
       </c>
       <c r="I78">
         <v>0.620284699014746</v>
@@ -6679,7 +6679,7 @@
         <v>126</v>
       </c>
       <c r="B79">
-        <v>123.225</v>
+        <v>24.6803151820088</v>
       </c>
       <c r="C79">
         <v>376099.907127143</v>
@@ -6691,13 +6691,13 @@
         <v>0.66199649737303</v>
       </c>
       <c r="F79">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G79">
-        <v>0.669203968318224</v>
+        <v>0.587142480054317</v>
       </c>
       <c r="H79">
-        <v>0.405761817812944</v>
+        <v>2.02590605635573</v>
       </c>
       <c r="I79">
         <v>0.682250889688753</v>
@@ -6756,7 +6756,7 @@
         <v>127</v>
       </c>
       <c r="B80">
-        <v>200.64</v>
+        <v>46.9106356844797</v>
       </c>
       <c r="C80">
         <v>784152.05342662</v>
@@ -6768,13 +6768,13 @@
         <v>1.0034516765286</v>
       </c>
       <c r="F80">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G80">
-        <v>1.08962535364876</v>
+        <v>1.11599980687395</v>
       </c>
       <c r="H80">
-        <v>0.249202551834131</v>
+        <v>1.0658563728767</v>
       </c>
       <c r="I80">
         <v>0.617369308151065</v>
@@ -6833,7 +6833,7 @@
         <v>128</v>
       </c>
       <c r="B81">
-        <v>110.122</v>
+        <v>24.6825060387548</v>
       </c>
       <c r="C81">
         <v>987514.071557479</v>
@@ -6845,13 +6845,13 @@
         <v>0.759818731117825</v>
       </c>
       <c r="F81">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G81">
-        <v>0.598044872380925</v>
+        <v>0.587194600339402</v>
       </c>
       <c r="H81">
-        <v>0.454041880823087</v>
+        <v>2.0257262338554</v>
       </c>
       <c r="I81">
         <v>0.576351329607065</v>
@@ -6910,7 +6910,7 @@
         <v>129</v>
       </c>
       <c r="B82">
-        <v>168.131</v>
+        <v>37.6845173789241</v>
       </c>
       <c r="C82">
         <v>1841096.51798489</v>
@@ -6922,13 +6922,13 @@
         <v>0.759818731117825</v>
       </c>
       <c r="F82">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G82">
-        <v>0.913077154776314</v>
+        <v>0.896511281575562</v>
       </c>
       <c r="H82">
-        <v>0.297387156443488</v>
+        <v>1.3268048386355</v>
       </c>
       <c r="I82">
         <v>0.547529317572646</v>
@@ -6987,7 +6987,7 @@
         <v>130</v>
       </c>
       <c r="B83">
-        <v>128.98</v>
+        <v>28.9092972237935</v>
       </c>
       <c r="C83">
         <v>603939.320198821</v>
@@ -6999,13 +6999,13 @@
         <v>0.759818731117825</v>
       </c>
       <c r="F83">
-        <v>184.136684529347</v>
+        <v>42.0346270631374</v>
       </c>
       <c r="G83">
-        <v>0.700457925207422</v>
+        <v>0.68774958275164</v>
       </c>
       <c r="H83">
-        <v>0.38765700108544</v>
+        <v>1.72954740521495</v>
       </c>
       <c r="I83">
         <v>0.469382331777597</v>

</xml_diff>

<commit_message>
separate multi hazard lulti return period data to an other demo
</commit_message>
<xml_diff>
--- a/inputs/all_data_compiled.xlsx
+++ b/inputs/all_data_compiled.xlsx
@@ -994,10 +994,10 @@
         <v>0.3</v>
       </c>
       <c r="V4">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W4">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X4">
         <v>1.5</v>
@@ -1071,10 +1071,10 @@
         <v>0.3</v>
       </c>
       <c r="V5">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W5">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X5">
         <v>1.5</v>
@@ -1148,10 +1148,10 @@
         <v>0.3</v>
       </c>
       <c r="V6">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W6">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X6">
         <v>1.5</v>
@@ -1225,10 +1225,10 @@
         <v>0.3</v>
       </c>
       <c r="V7">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W7">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X7">
         <v>1.5</v>
@@ -1302,10 +1302,10 @@
         <v>0.3</v>
       </c>
       <c r="V8">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W8">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X8">
         <v>1.5</v>
@@ -1379,10 +1379,10 @@
         <v>0.3</v>
       </c>
       <c r="V9">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W9">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X9">
         <v>1.5</v>
@@ -1456,10 +1456,10 @@
         <v>0.3</v>
       </c>
       <c r="V10">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W10">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X10">
         <v>1.5</v>
@@ -1533,10 +1533,10 @@
         <v>0.3</v>
       </c>
       <c r="V11">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W11">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X11">
         <v>1.5</v>
@@ -1610,10 +1610,10 @@
         <v>0.3</v>
       </c>
       <c r="V12">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W12">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X12">
         <v>1.5</v>
@@ -1687,10 +1687,10 @@
         <v>0.3</v>
       </c>
       <c r="V13">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W13">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X13">
         <v>1.5</v>
@@ -1761,10 +1761,10 @@
         <v>0.3</v>
       </c>
       <c r="V14">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W14">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X14">
         <v>1.5</v>
@@ -1838,10 +1838,10 @@
         <v>0.3</v>
       </c>
       <c r="V15">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W15">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X15">
         <v>1.5</v>
@@ -1915,10 +1915,10 @@
         <v>0.3</v>
       </c>
       <c r="V16">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W16">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X16">
         <v>1.5</v>
@@ -1992,10 +1992,10 @@
         <v>0.3</v>
       </c>
       <c r="V17">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W17">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X17">
         <v>1.5</v>
@@ -2069,10 +2069,10 @@
         <v>0.3</v>
       </c>
       <c r="V18">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W18">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X18">
         <v>1.5</v>
@@ -2146,10 +2146,10 @@
         <v>0.3</v>
       </c>
       <c r="V19">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W19">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X19">
         <v>1.5</v>
@@ -2223,10 +2223,10 @@
         <v>0.3</v>
       </c>
       <c r="V20">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W20">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X20">
         <v>1.5</v>
@@ -2300,10 +2300,10 @@
         <v>0.3</v>
       </c>
       <c r="V21">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W21">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X21">
         <v>1.5</v>
@@ -2377,10 +2377,10 @@
         <v>0.3</v>
       </c>
       <c r="V22">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W22">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X22">
         <v>1.5</v>
@@ -2454,10 +2454,10 @@
         <v>0.3</v>
       </c>
       <c r="V23">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W23">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X23">
         <v>1.5</v>
@@ -2531,10 +2531,10 @@
         <v>0.3</v>
       </c>
       <c r="V24">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W24">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X24">
         <v>1.5</v>
@@ -2608,10 +2608,10 @@
         <v>0.3</v>
       </c>
       <c r="V25">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W25">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X25">
         <v>1.5</v>
@@ -2685,10 +2685,10 @@
         <v>0.3</v>
       </c>
       <c r="V26">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W26">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X26">
         <v>1.5</v>
@@ -2762,10 +2762,10 @@
         <v>0.3</v>
       </c>
       <c r="V27">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W27">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X27">
         <v>1.5</v>
@@ -2839,10 +2839,10 @@
         <v>0.3</v>
       </c>
       <c r="V28">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W28">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X28">
         <v>1.5</v>
@@ -2916,10 +2916,10 @@
         <v>0.3</v>
       </c>
       <c r="V29">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W29">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X29">
         <v>1.5</v>
@@ -2993,10 +2993,10 @@
         <v>0.3</v>
       </c>
       <c r="V30">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W30">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X30">
         <v>1.5</v>
@@ -3070,10 +3070,10 @@
         <v>0.3</v>
       </c>
       <c r="V31">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W31">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X31">
         <v>1.5</v>
@@ -3147,10 +3147,10 @@
         <v>0.3</v>
       </c>
       <c r="V32">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W32">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X32">
         <v>1.5</v>
@@ -3209,10 +3209,10 @@
         <v>0.3</v>
       </c>
       <c r="V33">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W33">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X33">
         <v>1.5</v>
@@ -3286,10 +3286,10 @@
         <v>0.3</v>
       </c>
       <c r="V34">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W34">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X34">
         <v>1.5</v>
@@ -3363,10 +3363,10 @@
         <v>0.3</v>
       </c>
       <c r="V35">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W35">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X35">
         <v>1.5</v>
@@ -3440,10 +3440,10 @@
         <v>0.3</v>
       </c>
       <c r="V36">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W36">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X36">
         <v>1.5</v>
@@ -3517,10 +3517,10 @@
         <v>0.3</v>
       </c>
       <c r="V37">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W37">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X37">
         <v>1.5</v>
@@ -3594,10 +3594,10 @@
         <v>0.3</v>
       </c>
       <c r="V38">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W38">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X38">
         <v>1.5</v>
@@ -3671,10 +3671,10 @@
         <v>0.3</v>
       </c>
       <c r="V39">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W39">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X39">
         <v>1.5</v>
@@ -3748,10 +3748,10 @@
         <v>0.3</v>
       </c>
       <c r="V40">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W40">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X40">
         <v>1.5</v>
@@ -3825,10 +3825,10 @@
         <v>0.3</v>
       </c>
       <c r="V41">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W41">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X41">
         <v>1.5</v>
@@ -3902,10 +3902,10 @@
         <v>0.3</v>
       </c>
       <c r="V42">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W42">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X42">
         <v>1.5</v>
@@ -3979,10 +3979,10 @@
         <v>0.3</v>
       </c>
       <c r="V43">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W43">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X43">
         <v>1.5</v>
@@ -4056,10 +4056,10 @@
         <v>0.3</v>
       </c>
       <c r="V44">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W44">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X44">
         <v>1.5</v>
@@ -4133,10 +4133,10 @@
         <v>0.3</v>
       </c>
       <c r="V45">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W45">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X45">
         <v>1.5</v>
@@ -4210,10 +4210,10 @@
         <v>0.3</v>
       </c>
       <c r="V46">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W46">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X46">
         <v>1.5</v>
@@ -4287,10 +4287,10 @@
         <v>0.3</v>
       </c>
       <c r="V47">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W47">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X47">
         <v>1.5</v>
@@ -4364,10 +4364,10 @@
         <v>0.3</v>
       </c>
       <c r="V48">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W48">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X48">
         <v>1.5</v>
@@ -4441,10 +4441,10 @@
         <v>0.3</v>
       </c>
       <c r="V49">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W49">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X49">
         <v>1.5</v>
@@ -4515,10 +4515,10 @@
         <v>0.3</v>
       </c>
       <c r="V50">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W50">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X50">
         <v>1.5</v>
@@ -4592,10 +4592,10 @@
         <v>0.3</v>
       </c>
       <c r="V51">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W51">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X51">
         <v>1.5</v>
@@ -4669,10 +4669,10 @@
         <v>0.3</v>
       </c>
       <c r="V52">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W52">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X52">
         <v>1.5</v>
@@ -4746,10 +4746,10 @@
         <v>0.3</v>
       </c>
       <c r="V53">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W53">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X53">
         <v>1.5</v>
@@ -4820,10 +4820,10 @@
         <v>0.3</v>
       </c>
       <c r="V54">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W54">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X54">
         <v>1.5</v>
@@ -4897,10 +4897,10 @@
         <v>0.3</v>
       </c>
       <c r="V55">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W55">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X55">
         <v>1.5</v>
@@ -4974,10 +4974,10 @@
         <v>0.3</v>
       </c>
       <c r="V56">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W56">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X56">
         <v>1.5</v>
@@ -5051,10 +5051,10 @@
         <v>0.3</v>
       </c>
       <c r="V57">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W57">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X57">
         <v>1.5</v>
@@ -5128,10 +5128,10 @@
         <v>0.3</v>
       </c>
       <c r="V58">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W58">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X58">
         <v>1.5</v>
@@ -5205,10 +5205,10 @@
         <v>0.3</v>
       </c>
       <c r="V59">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W59">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X59">
         <v>1.5</v>
@@ -5282,10 +5282,10 @@
         <v>0.3</v>
       </c>
       <c r="V60">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W60">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X60">
         <v>1.5</v>
@@ -5359,10 +5359,10 @@
         <v>0.3</v>
       </c>
       <c r="V61">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W61">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X61">
         <v>1.5</v>
@@ -5436,10 +5436,10 @@
         <v>0.3</v>
       </c>
       <c r="V62">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W62">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X62">
         <v>1.5</v>
@@ -5513,10 +5513,10 @@
         <v>0.3</v>
       </c>
       <c r="V63">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W63">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X63">
         <v>1.5</v>
@@ -5590,10 +5590,10 @@
         <v>0.3</v>
       </c>
       <c r="V64">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W64">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X64">
         <v>1.5</v>
@@ -5667,10 +5667,10 @@
         <v>0.3</v>
       </c>
       <c r="V65">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W65">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X65">
         <v>1.5</v>
@@ -5744,10 +5744,10 @@
         <v>0.3</v>
       </c>
       <c r="V66">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W66">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X66">
         <v>1.5</v>
@@ -5821,10 +5821,10 @@
         <v>0.3</v>
       </c>
       <c r="V67">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W67">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X67">
         <v>1.5</v>
@@ -5898,10 +5898,10 @@
         <v>0.3</v>
       </c>
       <c r="V68">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W68">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X68">
         <v>1.5</v>
@@ -5975,10 +5975,10 @@
         <v>0.3</v>
       </c>
       <c r="V69">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W69">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X69">
         <v>1.5</v>
@@ -6049,10 +6049,10 @@
         <v>0.3</v>
       </c>
       <c r="V70">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W70">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X70">
         <v>1.5</v>
@@ -6126,10 +6126,10 @@
         <v>0.3</v>
       </c>
       <c r="V71">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W71">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X71">
         <v>1.5</v>
@@ -6203,10 +6203,10 @@
         <v>0.3</v>
       </c>
       <c r="V72">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W72">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X72">
         <v>1.5</v>
@@ -6280,10 +6280,10 @@
         <v>0.3</v>
       </c>
       <c r="V73">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W73">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X73">
         <v>1.5</v>
@@ -6357,10 +6357,10 @@
         <v>0.3</v>
       </c>
       <c r="V74">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W74">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X74">
         <v>1.5</v>
@@ -6434,10 +6434,10 @@
         <v>0.3</v>
       </c>
       <c r="V75">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W75">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X75">
         <v>1.5</v>
@@ -6511,10 +6511,10 @@
         <v>0.3</v>
       </c>
       <c r="V76">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W76">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X76">
         <v>1.5</v>
@@ -6585,10 +6585,10 @@
         <v>0.3</v>
       </c>
       <c r="V77">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W77">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X77">
         <v>1.5</v>
@@ -6662,10 +6662,10 @@
         <v>0.3</v>
       </c>
       <c r="V78">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W78">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X78">
         <v>1.5</v>
@@ -6739,10 +6739,10 @@
         <v>0.3</v>
       </c>
       <c r="V79">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W79">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X79">
         <v>1.5</v>
@@ -6816,10 +6816,10 @@
         <v>0.3</v>
       </c>
       <c r="V80">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W80">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X80">
         <v>1.5</v>
@@ -6893,10 +6893,10 @@
         <v>0.3</v>
       </c>
       <c r="V81">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W81">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X81">
         <v>1.5</v>
@@ -6970,10 +6970,10 @@
         <v>0.3</v>
       </c>
       <c r="V82">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W82">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X82">
         <v>1.5</v>
@@ -7047,10 +7047,10 @@
         <v>0.3</v>
       </c>
       <c r="V83">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="W83">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X83">
         <v>1.5</v>

</xml_diff>

<commit_message>
corrects income of poor households docs maps multi hazard multi rp demo
</commit_message>
<xml_diff>
--- a/inputs/all_data_compiled.xlsx
+++ b/inputs/all_data_compiled.xlsx
@@ -952,7 +952,7 @@
         <v>0.752295628751577</v>
       </c>
       <c r="H4">
-        <v>1.58115435053068</v>
+        <v>0.509131700870878</v>
       </c>
       <c r="I4">
         <v>0.693233188692644</v>
@@ -1029,7 +1029,7 @@
         <v>1.04025347212522</v>
       </c>
       <c r="H5">
-        <v>1.14346698969017</v>
+        <v>0.368196370680235</v>
       </c>
       <c r="I5">
         <v>0.496879896983716</v>
@@ -1106,7 +1106,7 @@
         <v>0.735047215279602</v>
       </c>
       <c r="H6">
-        <v>1.61825727866107</v>
+        <v>0.521078843728865</v>
       </c>
       <c r="I6">
         <v>0.475968914751725</v>
@@ -1183,7 +1183,7 @@
         <v>0.725964618985777</v>
       </c>
       <c r="H7">
-        <v>1.63850341349634</v>
+        <v>0.527598099145822</v>
       </c>
       <c r="I7">
         <v>0.660083320158597</v>
@@ -1260,7 +1260,7 @@
         <v>0.803939869564668</v>
       </c>
       <c r="H8">
-        <v>1.47958267939849</v>
+        <v>0.476425622766315</v>
       </c>
       <c r="I8">
         <v>0.551314358767217</v>
@@ -1337,7 +1337,7 @@
         <v>0.754437498166919</v>
       </c>
       <c r="H9">
-        <v>1.57666540856721</v>
+        <v>0.507686261558641</v>
       </c>
       <c r="I9">
         <v>0.437850462431834</v>
@@ -1414,7 +1414,7 @@
         <v>0.893224446045983</v>
       </c>
       <c r="H10">
-        <v>1.33168713815579</v>
+        <v>0.428803258486165</v>
       </c>
       <c r="I10">
         <v>0.261279700917478</v>
@@ -1491,7 +1491,7 @@
         <v>0.974692116016529</v>
       </c>
       <c r="H11">
-        <v>1.22038076100084</v>
+        <v>0.39296260504227</v>
       </c>
       <c r="I11">
         <v>0.573358263824997</v>
@@ -1568,7 +1568,7 @@
         <v>0.642616664059449</v>
       </c>
       <c r="H12">
-        <v>1.85101876875033</v>
+        <v>0.596028043537607</v>
       </c>
       <c r="I12">
         <v>0.538168398955</v>
@@ -1645,7 +1645,7 @@
         <v>1.54083508024529</v>
       </c>
       <c r="H13">
-        <v>0.771981065031574</v>
+        <v>0.248577902940167</v>
       </c>
       <c r="I13">
         <v>0.580481033452984</v>
@@ -1722,7 +1722,7 @@
         <v>1.62035401768068</v>
       </c>
       <c r="H14">
-        <v>0.734096063765355</v>
+        <v>0.236378932532444</v>
       </c>
       <c r="I14">
         <v>0.391077905964043</v>
@@ -1796,7 +1796,7 @@
         <v>1.18393037256222</v>
       </c>
       <c r="H15">
-        <v>1.00470055828664</v>
+        <v>0.323513579768298</v>
       </c>
       <c r="I15">
         <v>0.601053603455341</v>
@@ -1873,7 +1873,7 @@
         <v>1.70801067198868</v>
       </c>
       <c r="H16">
-        <v>0.696421589041249</v>
+        <v>0.224247751671282</v>
       </c>
       <c r="I16">
         <v>0.605775696080789</v>
@@ -1950,7 +1950,7 @@
         <v>1.18513102799471</v>
       </c>
       <c r="H17">
-        <v>1.00368269683939</v>
+        <v>0.323185828382284</v>
       </c>
       <c r="I17">
         <v>0.611077177703641</v>
@@ -2027,7 +2027,7 @@
         <v>0.803368247130913</v>
       </c>
       <c r="H18">
-        <v>1.48063545022328</v>
+        <v>0.476764614971897</v>
       </c>
       <c r="I18">
         <v>0.566535444651524</v>
@@ -2104,7 +2104,7 @@
         <v>0.793758299153181</v>
       </c>
       <c r="H19">
-        <v>1.49856134739602</v>
+        <v>0.48253675386152</v>
       </c>
       <c r="I19">
         <v>0.496198567578322</v>
@@ -2181,7 +2181,7 @@
         <v>1.40878845237852</v>
       </c>
       <c r="H20">
-        <v>0.84433933588644</v>
+        <v>0.271877266155434</v>
       </c>
       <c r="I20">
         <v>0.601417335117009</v>
@@ -2258,7 +2258,7 @@
         <v>0.918039948934714</v>
       </c>
       <c r="H21">
-        <v>1.2956903538523</v>
+        <v>0.417212293940441</v>
       </c>
       <c r="I21">
         <v>0.605970067589554</v>
@@ -2335,7 +2335,7 @@
         <v>0.756345802180509</v>
       </c>
       <c r="H22">
-        <v>1.57268739094804</v>
+        <v>0.506405339885269</v>
       </c>
       <c r="I22">
         <v>0.625601602025372</v>
@@ -2412,7 +2412,7 @@
         <v>0.770718794950339</v>
       </c>
       <c r="H23">
-        <v>1.54335863362773</v>
+        <v>0.49696148002813</v>
       </c>
       <c r="I23">
         <v>0.61358913909323</v>
@@ -2489,7 +2489,7 @@
         <v>0.851007317950554</v>
       </c>
       <c r="H24">
-        <v>1.3977500324561</v>
+        <v>0.450075510450865</v>
       </c>
       <c r="I24">
         <v>0.704419697775541</v>
@@ -2566,7 +2566,7 @@
         <v>1.07347293229032</v>
       </c>
       <c r="H25">
-        <v>1.10808150863004</v>
+        <v>0.356802245778873</v>
       </c>
       <c r="I25">
         <v>0.593455555845053</v>
@@ -2643,7 +2643,7 @@
         <v>1.22214530587667</v>
       </c>
       <c r="H26">
-        <v>0.973284846381268</v>
+        <v>0.313397720534768</v>
       </c>
       <c r="I26">
         <v>0.623269968447109</v>
@@ -2720,7 +2720,7 @@
         <v>1.52589398951219</v>
       </c>
       <c r="H27">
-        <v>0.779540069271806</v>
+        <v>0.251011902305521</v>
       </c>
       <c r="I27">
         <v>0.656626150696792</v>
@@ -2797,7 +2797,7 @@
         <v>1.12139047335289</v>
       </c>
       <c r="H28">
-        <v>1.0607326658744</v>
+        <v>0.341555918411556</v>
       </c>
       <c r="I28">
         <v>0.510060947320871</v>
@@ -2874,7 +2874,7 @@
         <v>0.773519451244686</v>
       </c>
       <c r="H29">
-        <v>1.53777064606679</v>
+        <v>0.495162148033505</v>
       </c>
       <c r="I29">
         <v>0.449828573348919</v>
@@ -2951,7 +2951,7 @@
         <v>0.877608517055713</v>
       </c>
       <c r="H30">
-        <v>1.35538281952459</v>
+        <v>0.436433267886918</v>
       </c>
       <c r="I30">
         <v>0.539234654715103</v>
@@ -3028,7 +3028,7 @@
         <v>1.06918159000258</v>
       </c>
       <c r="H31">
-        <v>1.11252898236201</v>
+        <v>0.358234332320567</v>
       </c>
       <c r="I31">
         <v>0.568224630141931</v>
@@ -3105,7 +3105,7 @@
         <v>0.546327207795047</v>
       </c>
       <c r="H32">
-        <v>2.17725840725839</v>
+        <v>0.701077207137202</v>
       </c>
       <c r="I32">
         <v>0.505140012725683</v>
@@ -3244,7 +3244,7 @@
         <v>0.64856441429642</v>
       </c>
       <c r="H34">
-        <v>1.83404374348254</v>
+        <v>0.590562085401378</v>
       </c>
       <c r="I34">
         <v>0.5052488202008</v>
@@ -3321,7 +3321,7 @@
         <v>0.985778885061004</v>
       </c>
       <c r="H35">
-        <v>1.20665549273979</v>
+        <v>0.388543068662213</v>
       </c>
       <c r="I35">
         <v>0.437850462431834</v>
@@ -3398,7 +3398,7 @@
         <v>0.838808950788161</v>
       </c>
       <c r="H36">
-        <v>1.41807679229948</v>
+        <v>0.456620727120433</v>
       </c>
       <c r="I36">
         <v>0.499190243762243</v>
@@ -3475,7 +3475,7 @@
         <v>1.00160245385094</v>
       </c>
       <c r="H37">
-        <v>1.18759244420021</v>
+        <v>0.382404767032467</v>
       </c>
       <c r="I37">
         <v>0.614787928154712</v>
@@ -3552,7 +3552,7 @@
         <v>0.91584393371999</v>
       </c>
       <c r="H38">
-        <v>1.2987971667337</v>
+        <v>0.418212687688251</v>
       </c>
       <c r="I38">
         <v>0.643920540702937</v>
@@ -3629,7 +3629,7 @@
         <v>1.13179240873424</v>
       </c>
       <c r="H39">
-        <v>1.0509838174441</v>
+        <v>0.338416789217001</v>
       </c>
       <c r="I39">
         <v>0.54518290933124</v>
@@ -3706,7 +3706,7 @@
         <v>0.869161116492157</v>
       </c>
       <c r="H40">
-        <v>1.36855582206259</v>
+        <v>0.440674974704156</v>
       </c>
       <c r="I40">
         <v>0.600693080642694</v>
@@ -3783,7 +3783,7 @@
         <v>0.958798775543336</v>
       </c>
       <c r="H41">
-        <v>1.24061016412093</v>
+        <v>0.39947647284694</v>
       </c>
       <c r="I41">
         <v>0.607822777429657</v>
@@ -3860,7 +3860,7 @@
         <v>1.07457945583464</v>
       </c>
       <c r="H42">
-        <v>1.10694048711537</v>
+        <v>0.356434836851148</v>
       </c>
       <c r="I42">
         <v>0.581058264319275</v>
@@ -3937,7 +3937,7 @@
         <v>1.34493954705693</v>
       </c>
       <c r="H43">
-        <v>0.884423027703129</v>
+        <v>0.284784214920408</v>
       </c>
       <c r="I43">
         <v>0.592091447554131</v>
@@ -4014,7 +4014,7 @@
         <v>0.896814157477256</v>
       </c>
       <c r="H44">
-        <v>1.32635674444728</v>
+        <v>0.427086871712025</v>
       </c>
       <c r="I44">
         <v>0.556690327994871</v>
@@ -4091,7 +4091,7 @@
         <v>0.628863068858177</v>
       </c>
       <c r="H45">
-        <v>1.89150160852271</v>
+        <v>0.609063517944311</v>
       </c>
       <c r="I45">
         <v>0.39129314485286</v>
@@ -4168,7 +4168,7 @@
         <v>0.889228342752476</v>
       </c>
       <c r="H46">
-        <v>1.33767160705186</v>
+        <v>0.430730257470699</v>
       </c>
       <c r="I46">
         <v>0.533733685257792</v>
@@ -4245,7 +4245,7 @@
         <v>0.668110726461808</v>
       </c>
       <c r="H47">
-        <v>1.78038678197118</v>
+        <v>0.573284543794721</v>
       </c>
       <c r="I47">
         <v>0.39129314485286</v>
@@ -4322,7 +4322,7 @@
         <v>0.913560192890968</v>
       </c>
       <c r="H48">
-        <v>1.30204393267355</v>
+        <v>0.419258146320885</v>
       </c>
       <c r="I48">
         <v>0.731612824879396</v>
@@ -4399,7 +4399,7 @@
         <v>0.64142774468548</v>
       </c>
       <c r="H49">
-        <v>1.85444972741088</v>
+        <v>0.597132812226305</v>
       </c>
       <c r="I49">
         <v>0.55283948979472</v>
@@ -4476,7 +4476,7 @@
         <v>0.633251917684749</v>
       </c>
       <c r="H50">
-        <v>1.87839226864834</v>
+        <v>0.604842310504766</v>
       </c>
       <c r="I50">
         <v>0.647841827821625</v>
@@ -4550,7 +4550,7 @@
         <v>1.1193729856901</v>
       </c>
       <c r="H51">
-        <v>1.06264446390265</v>
+        <v>0.342171517376654</v>
       </c>
       <c r="I51">
         <v>0.543458672242409</v>
@@ -4627,7 +4627,7 @@
         <v>0.686952016452318</v>
       </c>
       <c r="H52">
-        <v>1.73155544753879</v>
+        <v>0.55756085410749</v>
       </c>
       <c r="I52">
         <v>0.637626431996089</v>
@@ -4704,7 +4704,7 @@
         <v>0.883288623251905</v>
       </c>
       <c r="H53">
-        <v>1.34666684815495</v>
+        <v>0.433626725105894</v>
       </c>
       <c r="I53">
         <v>0.584921770775726</v>
@@ -4781,7 +4781,7 @@
         <v>0.790656005865207</v>
       </c>
       <c r="H54">
-        <v>1.50444124557571</v>
+        <v>0.484430081075378</v>
       </c>
       <c r="I54">
         <v>0.559499847441382</v>
@@ -4855,7 +4855,7 @@
         <v>0.717703374861577</v>
       </c>
       <c r="H55">
-        <v>1.65736367968896</v>
+        <v>0.533671104859845</v>
       </c>
       <c r="I55">
         <v>0.473517553705807</v>
@@ -4932,7 +4932,7 @@
         <v>0.685903660559299</v>
       </c>
       <c r="H56">
-        <v>1.73420200923819</v>
+        <v>0.558413046974698</v>
       </c>
       <c r="I56">
         <v>0.472971887518146</v>
@@ -5009,7 +5009,7 @@
         <v>0.943304621448199</v>
       </c>
       <c r="H57">
-        <v>1.26098768016169</v>
+        <v>0.406038033012065</v>
       </c>
       <c r="I57">
         <v>0.66171307823978</v>
@@ -5086,7 +5086,7 @@
         <v>1.09581604369203</v>
       </c>
       <c r="H58">
-        <v>1.08548831086476</v>
+        <v>0.349527236098453</v>
       </c>
       <c r="I58">
         <v>0.594974157700887</v>
@@ -5163,7 +5163,7 @@
         <v>1.0002212677612</v>
       </c>
       <c r="H59">
-        <v>1.18923236750226</v>
+        <v>0.382932822335729</v>
       </c>
       <c r="I59">
         <v>0.686160742512875</v>
@@ -5240,7 +5240,7 @@
         <v>0.860462822254108</v>
       </c>
       <c r="H60">
-        <v>1.38239035496003</v>
+        <v>0.44512969429713</v>
       </c>
       <c r="I60">
         <v>0.628316940328756</v>
@@ -5317,7 +5317,7 @@
         <v>0.79868850547439</v>
       </c>
       <c r="H61">
-        <v>1.48931091174181</v>
+        <v>0.479558113580863</v>
       </c>
       <c r="I61">
         <v>0.593796075486402</v>
@@ -5394,7 +5394,7 @@
         <v>1.31057112487762</v>
       </c>
       <c r="H62">
-        <v>0.907616140556154</v>
+        <v>0.292252397259082</v>
       </c>
       <c r="I62">
         <v>0.58379321753871</v>
@@ -5471,7 +5471,7 @@
         <v>0.949570481401407</v>
       </c>
       <c r="H63">
-        <v>1.25266689475253</v>
+        <v>0.403358740110315</v>
       </c>
       <c r="I63">
         <v>0.635505299806107</v>
@@ -5548,7 +5548,7 @@
         <v>0.966983738383891</v>
       </c>
       <c r="H64">
-        <v>1.2301091104942</v>
+        <v>0.396095133579134</v>
       </c>
       <c r="I64">
         <v>0.589964760829172</v>
@@ -5625,7 +5625,7 @@
         <v>1.02020300215156</v>
       </c>
       <c r="H65">
-        <v>1.16594001760157</v>
+        <v>0.375432685667706</v>
       </c>
       <c r="I65">
         <v>0.506628945908215</v>
@@ -5702,7 +5702,7 @@
         <v>1.58959574137969</v>
       </c>
       <c r="H66">
-        <v>0.748300637276083</v>
+        <v>0.240952805202899</v>
       </c>
       <c r="I66">
         <v>0.548077987002169</v>
@@ -5779,7 +5779,7 @@
         <v>0.728959819607431</v>
       </c>
       <c r="H67">
-        <v>1.63177101712732</v>
+        <v>0.525430267514998</v>
       </c>
       <c r="I67">
         <v>0.523882135324561</v>
@@ -5856,7 +5856,7 @@
         <v>0.672754423923139</v>
       </c>
       <c r="H68">
-        <v>1.76809763561163</v>
+        <v>0.569327438666946</v>
       </c>
       <c r="I68">
         <v>0.59513193838165</v>
@@ -5933,7 +5933,7 @@
         <v>0.564588008692948</v>
       </c>
       <c r="H69">
-        <v>2.10683806239441</v>
+        <v>0.678401856090999</v>
       </c>
       <c r="I69">
         <v>0.492333585156966</v>
@@ -6010,7 +6010,7 @@
         <v>0.575547804277705</v>
       </c>
       <c r="H70">
-        <v>2.066718867564</v>
+        <v>0.665483475355609</v>
       </c>
       <c r="I70">
         <v>0.566535444651524</v>
@@ -6084,7 +6084,7 @@
         <v>0.723063910953613</v>
       </c>
       <c r="H71">
-        <v>1.64507658073683</v>
+        <v>0.529714658997258</v>
       </c>
       <c r="I71">
         <v>0.603894799228239</v>
@@ -6161,7 +6161,7 @@
         <v>1.00329257875732</v>
       </c>
       <c r="H72">
-        <v>1.18559185173987</v>
+        <v>0.381760576260239</v>
       </c>
       <c r="I72">
         <v>0.554653565394186</v>
@@ -6238,7 +6238,7 @@
         <v>0.705881727442441</v>
       </c>
       <c r="H73">
-        <v>1.68512012712889</v>
+        <v>0.542608680935503</v>
       </c>
       <c r="I73">
         <v>0.612978966276617</v>
@@ -6315,7 +6315,7 @@
         <v>0.596313151847528</v>
       </c>
       <c r="H74">
-        <v>1.99474974281619</v>
+        <v>0.642309417186812</v>
       </c>
       <c r="I74">
         <v>0.595014685694195</v>
@@ -6392,7 +6392,7 @@
         <v>0.522536556848341</v>
       </c>
       <c r="H75">
-        <v>2.27638715549428</v>
+        <v>0.732996664069157</v>
       </c>
       <c r="I75">
         <v>0.62421925110961</v>
@@ -6469,7 +6469,7 @@
         <v>0.810526520526311</v>
       </c>
       <c r="H76">
-        <v>1.46755902017046</v>
+        <v>0.472554004494889</v>
       </c>
       <c r="I76">
         <v>0.561360301890219</v>
@@ -6546,7 +6546,7 @@
         <v>0.824461340295471</v>
       </c>
       <c r="H77">
-        <v>1.44275473954846</v>
+        <v>0.464567026134605</v>
       </c>
       <c r="I77">
         <v>0.57325688846045</v>
@@ -6620,7 +6620,7 @@
         <v>1.05899838133146</v>
       </c>
       <c r="H78">
-        <v>1.12322693523878</v>
+        <v>0.361679073146887</v>
       </c>
       <c r="I78">
         <v>0.620284699014746</v>
@@ -6697,7 +6697,7 @@
         <v>0.587142480054317</v>
       </c>
       <c r="H79">
-        <v>2.02590605635573</v>
+        <v>0.652341750146546</v>
       </c>
       <c r="I79">
         <v>0.682250889688753</v>
@@ -6774,7 +6774,7 @@
         <v>1.11599980687395</v>
       </c>
       <c r="H80">
-        <v>1.0658563728767</v>
+        <v>0.343205752066298</v>
       </c>
       <c r="I80">
         <v>0.617369308151065</v>
@@ -6851,7 +6851,7 @@
         <v>0.587194600339402</v>
       </c>
       <c r="H81">
-        <v>2.0257262338554</v>
+        <v>0.65228384730144</v>
       </c>
       <c r="I81">
         <v>0.576351329607065</v>
@@ -6928,7 +6928,7 @@
         <v>0.896511281575562</v>
       </c>
       <c r="H82">
-        <v>1.3268048386355</v>
+        <v>0.42723115804063</v>
       </c>
       <c r="I82">
         <v>0.547529317572646</v>
@@ -7005,7 +7005,7 @@
         <v>0.68774958275164</v>
       </c>
       <c r="H83">
-        <v>1.72954740521495</v>
+        <v>0.556914264479215</v>
       </c>
       <c r="I83">
         <v>0.469382331777597</v>

</xml_diff>

<commit_message>
corrects vr calculation (per Rio) and default is now welfare computed against local gdp, not national
</commit_message>
<xml_diff>
--- a/inputs/all_data_compiled.xlsx
+++ b/inputs/all_data_compiled.xlsx
@@ -958,7 +958,7 @@
         <v>0.178191030616645</v>
       </c>
       <c r="M4">
-        <v>0.166166503203906</v>
+        <v>0.15242128150753</v>
       </c>
       <c r="N4">
         <v>0.005</v>
@@ -1029,7 +1029,7 @@
         <v>0.218499680511182</v>
       </c>
       <c r="M5">
-        <v>0.185733320516112</v>
+        <v>0.14724254636513</v>
       </c>
       <c r="N5">
         <v>0.0350051202828125</v>
@@ -1100,7 +1100,7 @@
         <v>0.225682175386771</v>
       </c>
       <c r="M6">
-        <v>0.195585372223379</v>
+        <v>0.16585666659158</v>
       </c>
       <c r="N6">
         <v>0.0350051202828125</v>
@@ -1171,7 +1171,7 @@
         <v>0.270018647833677</v>
       </c>
       <c r="M7">
-        <v>0.237066768635532</v>
+        <v>0.206958140009178</v>
       </c>
       <c r="N7">
         <v>0.12786367</v>
@@ -1242,7 +1242,7 @@
         <v>0.238147011076631</v>
       </c>
       <c r="M8">
-        <v>0.195391798255078</v>
+        <v>0.151701628531602</v>
       </c>
       <c r="N8">
         <v>0.010690101</v>
@@ -1313,7 +1313,7 @@
         <v>0.279437373242884</v>
       </c>
       <c r="M9">
-        <v>0.208093362184809</v>
+        <v>0.181891571459366</v>
       </c>
       <c r="N9">
         <v>0.07587113385</v>
@@ -1384,7 +1384,7 @@
         <v>0.166754568414797</v>
       </c>
       <c r="M10">
-        <v>0.140280277344785</v>
+        <v>0.125986370157819</v>
       </c>
       <c r="N10">
         <v>0.005</v>
@@ -1455,7 +1455,7 @@
         <v>0.254441316756588</v>
       </c>
       <c r="M11">
-        <v>0.196826664779272</v>
+        <v>0.130239329179526</v>
       </c>
       <c r="N11">
         <v>0.0341985068</v>
@@ -1526,7 +1526,7 @@
         <v>0.252842799429658</v>
       </c>
       <c r="M12">
-        <v>0.211785792205617</v>
+        <v>0.171087536883518</v>
       </c>
       <c r="N12">
         <v>0.0145840769</v>
@@ -1597,7 +1597,7 @@
         <v>0.141498032602586</v>
       </c>
       <c r="M13">
-        <v>0.118237878280666</v>
+        <v>0.107909775226284</v>
       </c>
       <c r="N13">
         <v>0.0073847618</v>
@@ -1668,7 +1668,7 @@
         <v>0.1</v>
       </c>
       <c r="M14">
-        <v>0.150027442371021</v>
+        <v>0.216726125137212</v>
       </c>
       <c r="N14">
         <v>0.005</v>
@@ -1739,7 +1739,7 @@
         <v>0.179322416853919</v>
       </c>
       <c r="M15">
-        <v>0.13926162367626</v>
+        <v>0.117115029621362</v>
       </c>
       <c r="N15">
         <v>0.0057877453</v>
@@ -1810,7 +1810,7 @@
         <v>0.135012692833431</v>
       </c>
       <c r="M16">
-        <v>0.118552714094393</v>
+        <v>0.102282370153621</v>
       </c>
       <c r="N16">
         <v>0.005</v>
@@ -1881,7 +1881,7 @@
         <v>0.314776379217997</v>
       </c>
       <c r="M17">
-        <v>0.243638944526814</v>
+        <v>0.157837245475113</v>
       </c>
       <c r="N17">
         <v>0.089746621</v>
@@ -1952,7 +1952,7 @@
         <v>0.214752860823198</v>
       </c>
       <c r="M18">
-        <v>0.178424352239963</v>
+        <v>0.153647306539452</v>
       </c>
       <c r="N18">
         <v>0.0442099721</v>
@@ -2023,7 +2023,7 @@
         <v>0.169405846306724</v>
       </c>
       <c r="M19">
-        <v>0.138168293259434</v>
+        <v>0.126189427700763</v>
       </c>
       <c r="N19">
         <v>0.005</v>
@@ -2094,7 +2094,7 @@
         <v>0.202309529433378</v>
       </c>
       <c r="M20">
-        <v>0.141901567394898</v>
+        <v>0.116596190575278</v>
       </c>
       <c r="N20">
         <v>0.005</v>
@@ -2165,7 +2165,7 @@
         <v>0.204005020254989</v>
       </c>
       <c r="M21">
-        <v>0.15900694782868</v>
+        <v>0.130822279753631</v>
       </c>
       <c r="N21">
         <v>0.02495664335</v>
@@ -2236,7 +2236,7 @@
         <v>0.297789070997262</v>
       </c>
       <c r="M22">
-        <v>0.225439569296006</v>
+        <v>0.166789710102733</v>
       </c>
       <c r="N22">
         <v>0.07010183915</v>
@@ -2307,7 +2307,7 @@
         <v>0.243232687026165</v>
       </c>
       <c r="M23">
-        <v>0.201318212141033</v>
+        <v>0.163813413930527</v>
       </c>
       <c r="N23">
         <v>0.06113321225</v>
@@ -2378,7 +2378,7 @@
         <v>0.134164956387891</v>
       </c>
       <c r="M24">
-        <v>0.119222414974107</v>
+        <v>0.123894990624163</v>
       </c>
       <c r="N24">
         <v>0.04485040825</v>
@@ -2449,7 +2449,7 @@
         <v>0.296819050695959</v>
       </c>
       <c r="M25">
-        <v>0.236436827595109</v>
+        <v>0.198294078972812</v>
       </c>
       <c r="N25">
         <v>0.05838698235</v>
@@ -2520,7 +2520,7 @@
         <v>0.251871542495869</v>
       </c>
       <c r="M26">
-        <v>0.192457089631318</v>
+        <v>0.16071094980118</v>
       </c>
       <c r="N26">
         <v>0.03396154355</v>
@@ -2591,7 +2591,7 @@
         <v>0.15532452584697</v>
       </c>
       <c r="M27">
-        <v>0.127510337834153</v>
+        <v>0.108798222756118</v>
       </c>
       <c r="N27">
         <v>0.0590876739</v>
@@ -2662,7 +2662,7 @@
         <v>0.229680285340215</v>
       </c>
       <c r="M28">
-        <v>0.173800895887584</v>
+        <v>0.153195889727578</v>
       </c>
       <c r="N28">
         <v>0.04288886245</v>
@@ -2733,7 +2733,7 @@
         <v>0.205400793001962</v>
       </c>
       <c r="M29">
-        <v>0.166857064639412</v>
+        <v>0.148883898312743</v>
       </c>
       <c r="N29">
         <v>0.0103534937</v>
@@ -2804,7 +2804,7 @@
         <v>0.249399593150352</v>
       </c>
       <c r="M30">
-        <v>0.188155372709658</v>
+        <v>0.151198378718521</v>
       </c>
       <c r="N30">
         <v>0.0350051202828125</v>
@@ -2875,7 +2875,7 @@
         <v>0.181287404314544</v>
       </c>
       <c r="M31">
-        <v>0.151149087066025</v>
+        <v>0.14080956109018</v>
       </c>
       <c r="N31">
         <v>0.0350051202828125</v>
@@ -2946,7 +2946,7 @@
         <v>0.232153927323089</v>
       </c>
       <c r="M32">
-        <v>0.187558967096835</v>
+        <v>0.163991603714574</v>
       </c>
       <c r="N32">
         <v>0.0350051202828125</v>
@@ -3017,7 +3017,7 @@
         <v>0.253369958226559</v>
       </c>
       <c r="M33">
-        <v>0.181428246126104</v>
+        <v>0.133144632755999</v>
       </c>
       <c r="N33">
         <v>0.0350051202828125</v>
@@ -3088,7 +3088,7 @@
         <v>0.260595654757974</v>
       </c>
       <c r="M34">
-        <v>0.219040475797472</v>
+        <v>0.171221791961544</v>
       </c>
       <c r="N34">
         <v>0.02277472305</v>
@@ -3159,7 +3159,7 @@
         <v>0.237901665101841</v>
       </c>
       <c r="M35">
-        <v>0.188037982539166</v>
+        <v>0.1542390449639</v>
       </c>
       <c r="N35">
         <v>0.07116014505</v>
@@ -3230,7 +3230,7 @@
         <v>0.297998423955871</v>
       </c>
       <c r="M36">
-        <v>0.237875596174905</v>
+        <v>0.176569582409104</v>
       </c>
       <c r="N36">
         <v>0.10183898715</v>
@@ -3301,7 +3301,7 @@
         <v>0.122678929765886</v>
       </c>
       <c r="M37">
-        <v>0.120604314461909</v>
+        <v>0.11599043098252</v>
       </c>
       <c r="N37">
         <v>0.005</v>
@@ -3372,7 +3372,7 @@
         <v>0.14014806886094</v>
       </c>
       <c r="M38">
-        <v>0.11978516660878</v>
+        <v>0.119258567384796</v>
       </c>
       <c r="N38">
         <v>0.005</v>
@@ -3443,7 +3443,7 @@
         <v>0.176378914105142</v>
       </c>
       <c r="M39">
-        <v>0.134138472659734</v>
+        <v>0.113781081637163</v>
       </c>
       <c r="N39">
         <v>0.005</v>
@@ -3514,7 +3514,7 @@
         <v>0.257346197194046</v>
       </c>
       <c r="M40">
-        <v>0.189227295534466</v>
+        <v>0.17152392811848</v>
       </c>
       <c r="N40">
         <v>0.0350051202828125</v>
@@ -3585,7 +3585,7 @@
         <v>0.184630575867031</v>
       </c>
       <c r="M41">
-        <v>0.153514743624133</v>
+        <v>0.134264699279154</v>
       </c>
       <c r="N41">
         <v>0.005</v>
@@ -3656,7 +3656,7 @@
         <v>0.211067366579178</v>
       </c>
       <c r="M42">
-        <v>0.159383562958843</v>
+        <v>0.156583373378184</v>
       </c>
       <c r="N42">
         <v>0.0350051202828125</v>
@@ -3727,7 +3727,7 @@
         <v>0.16598090073096</v>
       </c>
       <c r="M43">
-        <v>0.142021390604446</v>
+        <v>0.127818871208354</v>
       </c>
       <c r="N43">
         <v>0.005</v>
@@ -3798,7 +3798,7 @@
         <v>0.174852863502603</v>
       </c>
       <c r="M44">
-        <v>0.134258497984096</v>
+        <v>0.121431696379744</v>
       </c>
       <c r="N44">
         <v>0.005</v>
@@ -3869,7 +3869,7 @@
         <v>0.140290999395078</v>
       </c>
       <c r="M45">
-        <v>0.122250793452255</v>
+        <v>0.112658594228783</v>
       </c>
       <c r="N45">
         <v>0.005</v>
@@ -3940,7 +3940,7 @@
         <v>0.16838593974175</v>
       </c>
       <c r="M46">
-        <v>0.145768053987649</v>
+        <v>0.121874471324649</v>
       </c>
       <c r="N46">
         <v>0.0350051202828125</v>
@@ -4011,7 +4011,7 @@
         <v>0.13800893547045</v>
       </c>
       <c r="M47">
-        <v>0.135719339804403</v>
+        <v>0.130257361938168</v>
       </c>
       <c r="N47">
         <v>0.0350051202828125</v>
@@ -4082,7 +4082,7 @@
         <v>0.235886741559019</v>
       </c>
       <c r="M48">
-        <v>0.185826502892695</v>
+        <v>0.153015407242403</v>
       </c>
       <c r="N48">
         <v>0.1360574775</v>
@@ -4153,7 +4153,7 @@
         <v>0.26952277904328</v>
       </c>
       <c r="M49">
-        <v>0.239063205159925</v>
+        <v>0.220262356843528</v>
       </c>
       <c r="N49">
         <v>0.08391870735</v>
@@ -4224,7 +4224,7 @@
         <v>0.136136094262009</v>
       </c>
       <c r="M50">
-        <v>0.119562229407199</v>
+        <v>0.112270576613113</v>
       </c>
       <c r="N50">
         <v>0.0350051202828125</v>
@@ -4295,7 +4295,7 @@
         <v>0.208906850820058</v>
       </c>
       <c r="M51">
-        <v>0.178106591316575</v>
+        <v>0.144329833534141</v>
       </c>
       <c r="N51">
         <v>0.0507989316</v>
@@ -4366,7 +4366,7 @@
         <v>0.306455152737199</v>
       </c>
       <c r="M52">
-        <v>0.247125558807786</v>
+        <v>0.193198501872659</v>
       </c>
       <c r="N52">
         <v>0.0425295093</v>
@@ -4437,7 +4437,7 @@
         <v>0.280360319783808</v>
       </c>
       <c r="M53">
-        <v>0.220475071118056</v>
+        <v>0.17835053914082</v>
       </c>
       <c r="N53">
         <v>0.061471479</v>
@@ -4508,7 +4508,7 @@
         <v>0.211017429502622</v>
       </c>
       <c r="M54">
-        <v>0.18436708049434</v>
+        <v>0.154132021167951</v>
       </c>
       <c r="N54">
         <v>0.089146712</v>
@@ -4579,7 +4579,7 @@
         <v>0.127832255372418</v>
       </c>
       <c r="M55">
-        <v>0.117120789011774</v>
+        <v>0.105328963340617</v>
       </c>
       <c r="N55">
         <v>0.005</v>
@@ -4650,7 +4650,7 @@
         <v>0.211085835608129</v>
       </c>
       <c r="M56">
-        <v>0.151519363952184</v>
+        <v>0.112404011864711</v>
       </c>
       <c r="N56">
         <v>0.0350051202828125</v>
@@ -4721,7 +4721,7 @@
         <v>0.189127340413884</v>
       </c>
       <c r="M57">
-        <v>0.151106009378652</v>
+        <v>0.113205689192865</v>
       </c>
       <c r="N57">
         <v>0.0350051202828125</v>
@@ -4792,7 +4792,7 @@
         <v>0.146760294970586</v>
       </c>
       <c r="M58">
-        <v>0.126311962639249</v>
+        <v>0.108188043797672</v>
       </c>
       <c r="N58">
         <v>0.0350051202828125</v>
@@ -4863,7 +4863,7 @@
         <v>0.265662880856176</v>
       </c>
       <c r="M59">
-        <v>0.202156069578703</v>
+        <v>0.17187298757124</v>
       </c>
       <c r="N59">
         <v>0.05413932165</v>
@@ -4934,7 +4934,7 @@
         <v>0.277240189769794</v>
       </c>
       <c r="M60">
-        <v>0.209949405885033</v>
+        <v>0.179002925547794</v>
       </c>
       <c r="N60">
         <v>0.02260134445</v>
@@ -5005,7 +5005,7 @@
         <v>0.305753634128874</v>
       </c>
       <c r="M61">
-        <v>0.256353364420662</v>
+        <v>0.204158284530675</v>
       </c>
       <c r="N61">
         <v>0.0816000164</v>
@@ -5076,7 +5076,7 @@
         <v>0.195406831344331</v>
       </c>
       <c r="M62">
-        <v>0.154017767286415</v>
+        <v>0.126151476726511</v>
       </c>
       <c r="N62">
         <v>0.005</v>
@@ -5147,7 +5147,7 @@
         <v>0.169807805452049</v>
       </c>
       <c r="M63">
-        <v>0.15257997056861</v>
+        <v>0.11108931349105</v>
       </c>
       <c r="N63">
         <v>0.005</v>
@@ -5218,7 +5218,7 @@
         <v>0.286705825555198</v>
       </c>
       <c r="M64">
-        <v>0.244486100381733</v>
+        <v>0.188862504264756</v>
       </c>
       <c r="N64">
         <v>0.04228809785</v>
@@ -5289,7 +5289,7 @@
         <v>0.30737421063353</v>
       </c>
       <c r="M65">
-        <v>0.227245200740819</v>
+        <v>0.155836855895197</v>
       </c>
       <c r="N65">
         <v>0.06469784885</v>
@@ -5360,7 +5360,7 @@
         <v>0.347250157133878</v>
       </c>
       <c r="M66">
-        <v>0.294055150477263</v>
+        <v>0.249450371632919</v>
       </c>
       <c r="N66">
         <v>0.08165578565</v>
@@ -5431,7 +5431,7 @@
         <v>0.203654811642032</v>
       </c>
       <c r="M67">
-        <v>0.155857088502843</v>
+        <v>0.115122358895172</v>
       </c>
       <c r="N67">
         <v>0.005</v>
@@ -5502,7 +5502,7 @@
         <v>0.194472942180233</v>
       </c>
       <c r="M68">
-        <v>0.154985043003113</v>
+        <v>0.137066537445382</v>
       </c>
       <c r="N68">
         <v>0.00881345625</v>
@@ -5573,7 +5573,7 @@
         <v>0.254750167334233</v>
       </c>
       <c r="M69">
-        <v>0.203241966135687</v>
+        <v>0.160280920637414</v>
       </c>
       <c r="N69">
         <v>0.029992736</v>
@@ -5644,7 +5644,7 @@
         <v>0.12816241940436</v>
       </c>
       <c r="M70">
-        <v>0.112184030662227</v>
+        <v>0.109007161915461</v>
       </c>
       <c r="N70">
         <v>0.005</v>
@@ -5715,7 +5715,7 @@
         <v>0.168555226984694</v>
       </c>
       <c r="M71">
-        <v>0.125702608662488</v>
+        <v>0.109811425134469</v>
       </c>
       <c r="N71">
         <v>0.005</v>
@@ -5786,7 +5786,7 @@
         <v>0.282250521071628</v>
       </c>
       <c r="M72">
-        <v>0.225282359744661</v>
+        <v>0.178461879432624</v>
       </c>
       <c r="N72">
         <v>0.0615011812</v>
@@ -5857,7 +5857,7 @@
         <v>0.262003894306099</v>
       </c>
       <c r="M73">
-        <v>0.218566528818886</v>
+        <v>0.180139223905763</v>
       </c>
       <c r="N73">
         <v>0.0350051202828125</v>
@@ -5928,7 +5928,7 @@
         <v>0.303288852817938</v>
       </c>
       <c r="M74">
-        <v>0.240386991952715</v>
+        <v>0.199160191128915</v>
       </c>
       <c r="N74">
         <v>0.01768973355</v>
@@ -5999,7 +5999,7 @@
         <v>0.207003196089491</v>
       </c>
       <c r="M75">
-        <v>0.148394266060731</v>
+        <v>0.144174295565331</v>
       </c>
       <c r="N75">
         <v>0.0979669383</v>
@@ -6070,7 +6070,7 @@
         <v>0.25551228042286</v>
       </c>
       <c r="M76">
-        <v>0.234490036446755</v>
+        <v>0.18881789715651</v>
       </c>
       <c r="N76">
         <v>0.04003645535</v>
@@ -6141,7 +6141,7 @@
         <v>0.26063054979374</v>
       </c>
       <c r="M77">
-        <v>0.190984364814419</v>
+        <v>0.15545908567038</v>
       </c>
       <c r="N77">
         <v>0.005</v>
@@ -6212,7 +6212,7 @@
         <v>0.202182502351834</v>
       </c>
       <c r="M78">
-        <v>0.153070766444893</v>
+        <v>0.137361819211783</v>
       </c>
       <c r="N78">
         <v>0.02386936895</v>
@@ -6283,7 +6283,7 @@
         <v>0.279118461019237</v>
       </c>
       <c r="M79">
-        <v>0.21804373286126</v>
+        <v>0.175768657603379</v>
       </c>
       <c r="N79">
         <v>0.0106582598</v>
@@ -6354,7 +6354,7 @@
         <v>0.280778306486212</v>
       </c>
       <c r="M80">
-        <v>0.273994126283698</v>
+        <v>0.26537811714166</v>
       </c>
       <c r="N80">
         <v>0.0350051202828125</v>
@@ -6425,7 +6425,7 @@
         <v>0.268755158184319</v>
       </c>
       <c r="M81">
-        <v>0.219903491041796</v>
+        <v>0.185302806499261</v>
       </c>
       <c r="N81">
         <v>0.0350051202828125</v>
@@ -6496,7 +6496,7 @@
         <v>0.251052461139896</v>
       </c>
       <c r="M82">
-        <v>0.22087205743708</v>
+        <v>0.180356271635341</v>
       </c>
       <c r="N82">
         <v>0.0350051202828125</v>
@@ -6567,7 +6567,7 @@
         <v>0.187990989196993</v>
       </c>
       <c r="M83">
-        <v>0.152448701250473</v>
+        <v>0.124954676418872</v>
       </c>
       <c r="N83">
         <v>0.005</v>
@@ -6638,7 +6638,7 @@
         <v>0.12640871784261</v>
       </c>
       <c r="M84">
-        <v>0.142820971329391</v>
+        <v>0.15930999050001</v>
       </c>
       <c r="N84">
         <v>0.0350051202828125</v>
@@ -6709,7 +6709,7 @@
         <v>0.21589049716803</v>
       </c>
       <c r="M85">
-        <v>0.1579790637339</v>
+        <v>0.126452227767051</v>
       </c>
       <c r="N85">
         <v>0.013158047</v>
@@ -6780,7 +6780,7 @@
         <v>0.26403522249323</v>
       </c>
       <c r="M86">
-        <v>0.208911373690105</v>
+        <v>0.165919371829714</v>
       </c>
       <c r="N86">
         <v>0.0350051202828125</v>
@@ -6851,7 +6851,7 @@
         <v>0.288167055592367</v>
       </c>
       <c r="M87">
-        <v>0.2358938796033</v>
+        <v>0.190818921327535</v>
       </c>
       <c r="N87">
         <v>0.0350051202828125</v>
@@ -6922,7 +6922,7 @@
         <v>0.319917414799965</v>
       </c>
       <c r="M88">
-        <v>0.253115925958439</v>
+        <v>0.190569579519451</v>
       </c>
       <c r="N88">
         <v>0.00890518715</v>

</xml_diff>

<commit_message>
remove duplicate pho thu (25) from raw data
</commit_message>
<xml_diff>
--- a/inputs/all_data_compiled.xlsx
+++ b/inputs/all_data_compiled.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
   <si>
     <t>description</t>
   </si>
@@ -701,7 +701,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W67"/>
+  <dimension ref="A1:W66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -862,10 +862,10 @@
         <v>6698811</v>
       </c>
       <c r="C4">
-        <v>601.835764693321</v>
+        <v>595.028750754764</v>
       </c>
       <c r="D4">
-        <v>5268.98375025418</v>
+        <v>5269.41787104803</v>
       </c>
       <c r="E4">
         <v>0.0599520392715931</v>
@@ -874,7 +874,7 @@
         <v>4989.1787109375</v>
       </c>
       <c r="G4">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H4">
         <v>0.132860738784075</v>
@@ -933,10 +933,10 @@
         <v>774681</v>
       </c>
       <c r="C5">
-        <v>245.646227649306</v>
+        <v>242.867866186499</v>
       </c>
       <c r="D5">
-        <v>5193.75705347368</v>
+        <v>5198.65574387884</v>
       </c>
       <c r="E5">
         <v>0.638095259666443</v>
@@ -945,7 +945,7 @@
         <v>2036.39099121094</v>
       </c>
       <c r="G5">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H5">
         <v>0.108243891969323</v>
@@ -1004,10 +1004,10 @@
         <v>540048</v>
       </c>
       <c r="C6">
-        <v>247.407867971581</v>
+        <v>244.609581620736</v>
       </c>
       <c r="D6">
-        <v>4246.66624803465</v>
+        <v>4250.07285787509</v>
       </c>
       <c r="E6">
         <v>0.549019634723663</v>
@@ -1016,7 +1016,7 @@
         <v>2050.99487304688</v>
       </c>
       <c r="G6">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H6">
         <v>0.130565547384322</v>
@@ -1075,10 +1075,10 @@
         <v>311681</v>
       </c>
       <c r="C7">
-        <v>267.005595655593</v>
+        <v>263.985650816943</v>
       </c>
       <c r="D7">
-        <v>6671.46408314999</v>
+        <v>6678.38073062415</v>
       </c>
       <c r="E7">
         <v>0.696078419685364</v>
@@ -1087,7 +1087,7 @@
         <v>2213.45874023438</v>
       </c>
       <c r="G7">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H7">
         <v>0.0653125615790486</v>
@@ -1146,10 +1146,10 @@
         <v>772231</v>
       </c>
       <c r="C8">
-        <v>307.017677002576</v>
+        <v>303.545178807316</v>
       </c>
       <c r="D8">
-        <v>4314.00773944852</v>
+        <v>4316.75213324026</v>
       </c>
       <c r="E8">
         <v>0.44144144654274</v>
@@ -1158,7 +1158,7 @@
         <v>2545.15625</v>
       </c>
       <c r="G8">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H8">
         <v>0.0747878458350897</v>
@@ -1217,10 +1217,10 @@
         <v>655299</v>
       </c>
       <c r="C9">
-        <v>300.159185009219</v>
+        <v>296.764259223801</v>
       </c>
       <c r="D9">
-        <v>4855.06413733978</v>
+        <v>4858.73619990682</v>
       </c>
       <c r="E9">
         <v>0.519607841968536</v>
@@ -1229,7 +1229,7 @@
         <v>2488.2998046875</v>
       </c>
       <c r="G9">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H9">
         <v>0.086600043810904</v>
@@ -1288,10 +1288,10 @@
         <v>522590</v>
       </c>
       <c r="C10">
-        <v>299.22346221974</v>
+        <v>295.839119850005</v>
       </c>
       <c r="D10">
-        <v>5465.50623370859</v>
+        <v>5470.13743953441</v>
       </c>
       <c r="E10">
         <v>0.577777802944183</v>
@@ -1300,7 +1300,7 @@
         <v>2480.54272460938</v>
       </c>
       <c r="G10">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H10">
         <v>0.14007131755352</v>
@@ -1359,10 +1359,10 @@
         <v>395457</v>
       </c>
       <c r="C11">
-        <v>200.90596758438</v>
+        <v>198.63363715486</v>
       </c>
       <c r="D11">
-        <v>5777.61812007435</v>
+        <v>5783.99812382942</v>
       </c>
       <c r="E11">
         <v>0.73737370967865</v>
@@ -1371,7 +1371,7 @@
         <v>1665.49719238281</v>
       </c>
       <c r="G11">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H11">
         <v>0.0966347008943558</v>
@@ -1430,10 +1430,10 @@
         <v>1145579</v>
       </c>
       <c r="C12">
-        <v>315.903200245013</v>
+        <v>312.330203069615</v>
       </c>
       <c r="D12">
-        <v>6623.88389619403</v>
+        <v>6630.0978049085</v>
       </c>
       <c r="E12">
         <v>0.634920656681061</v>
@@ -1442,7 +1442,7 @@
         <v>2618.81665039062</v>
       </c>
       <c r="G12">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H12">
         <v>0.0685315057635307</v>
@@ -1501,10 +1501,10 @@
         <v>789998</v>
       </c>
       <c r="C13">
-        <v>280.689271409691</v>
+        <v>277.514558481384</v>
       </c>
       <c r="D13">
-        <v>3815.04551707491</v>
+        <v>3817.3543992343</v>
       </c>
       <c r="E13">
         <v>0.421052634716034</v>
@@ -1513,7 +1513,7 @@
         <v>2326.8955078125</v>
       </c>
       <c r="G13">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H13">
         <v>0.108779340982437</v>
@@ -1572,10 +1572,10 @@
         <v>814113</v>
       </c>
       <c r="C14">
-        <v>298.437464500658</v>
+        <v>295.062012093507</v>
       </c>
       <c r="D14">
-        <v>4727.31610324083</v>
+        <v>4730.81210788535</v>
       </c>
       <c r="E14">
         <v>0.508771955966949</v>
@@ -1584,7 +1584,7 @@
         <v>2474.02685546875</v>
       </c>
       <c r="G14">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H14">
         <v>0.104054864495993</v>
@@ -1643,10 +1643,10 @@
         <v>1201300</v>
       </c>
       <c r="C15">
-        <v>402.232749789315</v>
+        <v>397.683329341104</v>
       </c>
       <c r="D15">
-        <v>4356.73529099745</v>
+        <v>4358.32132753263</v>
       </c>
       <c r="E15">
         <v>0.258503407239914</v>
@@ -1655,7 +1655,7 @@
         <v>3334.48291015625</v>
       </c>
       <c r="G15">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H15">
         <v>0.098390681669116</v>
@@ -1714,10 +1714,10 @@
         <v>779760</v>
       </c>
       <c r="C16">
-        <v>237.483649140955</v>
+        <v>234.797609851307</v>
       </c>
       <c r="D16">
-        <v>3801.80172635352</v>
+        <v>3804.64576828394</v>
       </c>
       <c r="E16">
         <v>0.514285743236542</v>
@@ -1726,7 +1726,7 @@
         <v>1968.72375488281</v>
       </c>
       <c r="G16">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H16">
         <v>0.0929199308156967</v>
@@ -1785,10 +1785,10 @@
         <v>1206649</v>
       </c>
       <c r="C17">
-        <v>522.968702317192</v>
+        <v>517.053707803836</v>
       </c>
       <c r="D17">
-        <v>4970.77722207547</v>
+        <v>4971.76305454578</v>
       </c>
       <c r="E17">
         <v>0.142857149243355</v>
@@ -1797,7 +1797,7 @@
         <v>4335.3759765625</v>
       </c>
       <c r="G17">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H17">
         <v>0.137298237532377</v>
@@ -1856,10 +1856,10 @@
         <v>1660898</v>
       </c>
       <c r="C18">
-        <v>409.266706371464</v>
+        <v>404.637728935606</v>
       </c>
       <c r="D18">
-        <v>4621.3051022748</v>
+        <v>4623.21115171556</v>
       </c>
       <c r="E18">
         <v>0.291666656732559</v>
@@ -1868,7 +1868,7 @@
         <v>3392.7939453125</v>
       </c>
       <c r="G18">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H18">
         <v>0.174647849053144</v>
@@ -1927,43 +1927,43 @@
         <v>1409905</v>
       </c>
       <c r="C19">
-        <v>325.830378825752</v>
+        <v>327.624163568227</v>
       </c>
       <c r="D19">
-        <v>2840.83477201691</v>
+        <v>4255.63799053413</v>
       </c>
       <c r="E19">
-        <v>0.0555555559694767</v>
+        <v>0.384057968854904</v>
       </c>
       <c r="F19">
-        <v>2701.1123046875</v>
+        <v>2747.05297851562</v>
       </c>
       <c r="G19">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H19">
-        <v>0.11145331710577</v>
+        <v>0.261015903204679</v>
       </c>
       <c r="I19">
-        <v>0.11145331710577</v>
+        <v>0.261015903204679</v>
       </c>
       <c r="J19">
-        <v>0.0333333333333333</v>
+        <v>0.0861635209601078</v>
       </c>
       <c r="K19">
         <v>0.0333333333333333</v>
       </c>
       <c r="L19">
-        <v>1</v>
+        <v>0.847826086956522</v>
       </c>
       <c r="M19">
-        <v>1</v>
+        <v>0.847826086956522</v>
       </c>
       <c r="N19">
         <v>0.321292266730143</v>
       </c>
       <c r="O19">
-        <v>0.290998182711012</v>
+        <v>0.274841338084031</v>
       </c>
       <c r="P19">
         <v>8.22366</v>
@@ -1992,52 +1992,52 @@
     </row>
     <row r="20" spans="1:23">
       <c r="A20" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B20">
-        <v>1409905</v>
+        <v>1268179</v>
       </c>
       <c r="C20">
-        <v>331.372120696666</v>
+        <v>386.820155474218</v>
       </c>
       <c r="D20">
-        <v>4253.30102905185</v>
+        <v>3892.61984932241</v>
       </c>
       <c r="E20">
-        <v>0.384057968854904</v>
+        <v>0.185185179114342</v>
       </c>
       <c r="F20">
-        <v>2747.05297851562</v>
+        <v>3243.39770507812</v>
       </c>
       <c r="G20">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H20">
-        <v>0.261015903204679</v>
+        <v>0.179372223094106</v>
       </c>
       <c r="I20">
-        <v>0.261015903204679</v>
+        <v>0.179372223094106</v>
       </c>
       <c r="J20">
-        <v>0.0861635209601078</v>
+        <v>0.0333333333333333</v>
       </c>
       <c r="K20">
         <v>0.0333333333333333</v>
       </c>
       <c r="L20">
-        <v>0.847826086956522</v>
+        <v>0.97037037037037</v>
       </c>
       <c r="M20">
-        <v>0.847826086956522</v>
+        <v>0.97037037037037</v>
       </c>
       <c r="N20">
-        <v>0.321292266730143</v>
+        <v>0.576737087466279</v>
       </c>
       <c r="O20">
-        <v>0.274841338084031</v>
+        <v>0.513706271526953</v>
       </c>
       <c r="P20">
-        <v>8.22366</v>
+        <v>8.50046</v>
       </c>
       <c r="Q20">
         <v>0.2697</v>
@@ -2063,31 +2063,31 @@
     </row>
     <row r="21" spans="1:23">
       <c r="A21" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B21">
-        <v>1268179</v>
+        <v>1084891</v>
       </c>
       <c r="C21">
-        <v>391.245303312349</v>
+        <v>600.059496370441</v>
       </c>
       <c r="D21">
-        <v>3891.61413394511</v>
+        <v>5415.173828975</v>
       </c>
       <c r="E21">
-        <v>0.185185179114342</v>
+        <v>0.0797101482748985</v>
       </c>
       <c r="F21">
-        <v>3243.39770507812</v>
+        <v>5031.3603515625</v>
       </c>
       <c r="G21">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H21">
-        <v>0.179372223094106</v>
+        <v>0.221526484936476</v>
       </c>
       <c r="I21">
-        <v>0.179372223094106</v>
+        <v>0.221526484936476</v>
       </c>
       <c r="J21">
         <v>0.0333333333333333</v>
@@ -2096,19 +2096,19 @@
         <v>0.0333333333333333</v>
       </c>
       <c r="L21">
-        <v>0.97037037037037</v>
+        <v>0.949275362318841</v>
       </c>
       <c r="M21">
-        <v>0.97037037037037</v>
+        <v>0.949275362318841</v>
       </c>
       <c r="N21">
-        <v>0.576737087466279</v>
+        <v>0.366131488005726</v>
       </c>
       <c r="O21">
-        <v>0.513706271526953</v>
+        <v>0.330703505887772</v>
       </c>
       <c r="P21">
-        <v>8.50046</v>
+        <v>6.93767</v>
       </c>
       <c r="Q21">
         <v>0.2697</v>
@@ -2134,31 +2134,31 @@
     </row>
     <row r="22" spans="1:23">
       <c r="A22" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B22">
-        <v>1084891</v>
+        <v>1825318</v>
       </c>
       <c r="C22">
-        <v>606.924061066813</v>
+        <v>392.630658507522</v>
       </c>
       <c r="D22">
-        <v>5414.57926035212</v>
+        <v>3953.74531654058</v>
       </c>
       <c r="E22">
-        <v>0.0797101482748985</v>
+        <v>0.185792356729507</v>
       </c>
       <c r="F22">
-        <v>5031.3603515625</v>
+        <v>3292.11743164062</v>
       </c>
       <c r="G22">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H22">
-        <v>0.221526484936476</v>
+        <v>0.229850724339485</v>
       </c>
       <c r="I22">
-        <v>0.221526484936476</v>
+        <v>0.229850724339485</v>
       </c>
       <c r="J22">
         <v>0.0333333333333333</v>
@@ -2167,19 +2167,19 @@
         <v>0.0333333333333333</v>
       </c>
       <c r="L22">
-        <v>0.949275362318841</v>
+        <v>0.896174863387978</v>
       </c>
       <c r="M22">
-        <v>0.949275362318841</v>
+        <v>0.896174863387978</v>
       </c>
       <c r="N22">
-        <v>0.366131488005726</v>
+        <v>0.75982113587613</v>
       </c>
       <c r="O22">
-        <v>0.330703505887772</v>
+        <v>0.676719386866709</v>
       </c>
       <c r="P22">
-        <v>6.93767</v>
+        <v>10.0686</v>
       </c>
       <c r="Q22">
         <v>0.2697</v>
@@ -2205,31 +2205,31 @@
     </row>
     <row r="23" spans="1:23">
       <c r="A23" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B23">
-        <v>1825318</v>
+        <v>1941369</v>
       </c>
       <c r="C23">
-        <v>397.122277377662</v>
+        <v>509.439338768411</v>
       </c>
       <c r="D23">
-        <v>3952.72038332814</v>
+        <v>4462.82405305482</v>
       </c>
       <c r="E23">
-        <v>0.185792356729507</v>
+        <v>0.0483870953321457</v>
       </c>
       <c r="F23">
-        <v>3292.11743164062</v>
+        <v>4271.53125</v>
       </c>
       <c r="G23">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H23">
-        <v>0.229850724339485</v>
+        <v>0.290047507733107</v>
       </c>
       <c r="I23">
-        <v>0.229850724339485</v>
+        <v>0.290047507733107</v>
       </c>
       <c r="J23">
         <v>0.0333333333333333</v>
@@ -2238,19 +2238,19 @@
         <v>0.0333333333333333</v>
       </c>
       <c r="L23">
-        <v>0.896174863387978</v>
+        <v>0.913978494623656</v>
       </c>
       <c r="M23">
-        <v>0.896174863387978</v>
+        <v>0.913978494623656</v>
       </c>
       <c r="N23">
-        <v>0.75982113587613</v>
+        <v>0.808409112789193</v>
       </c>
       <c r="O23">
-        <v>0.676719386866709</v>
+        <v>0.732759824454356</v>
       </c>
       <c r="P23">
-        <v>10.0686</v>
+        <v>6.50645</v>
       </c>
       <c r="Q23">
         <v>0.2697</v>
@@ -2276,31 +2276,31 @@
     </row>
     <row r="24" spans="1:23">
       <c r="A24" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B24">
-        <v>1941369</v>
+        <v>1210637</v>
       </c>
       <c r="C24">
-        <v>515.267226371233</v>
+        <v>381.500218272586</v>
       </c>
       <c r="D24">
-        <v>4462.52771979616</v>
+        <v>3426.6603769444</v>
       </c>
       <c r="E24">
-        <v>0.0483870953321457</v>
+        <v>0.0748299285769463</v>
       </c>
       <c r="F24">
-        <v>4271.53125</v>
+        <v>3198.79125976562</v>
       </c>
       <c r="G24">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H24">
-        <v>0.290047507733107</v>
+        <v>0.204068381339312</v>
       </c>
       <c r="I24">
-        <v>0.290047507733107</v>
+        <v>0.204068381339312</v>
       </c>
       <c r="J24">
         <v>0.0333333333333333</v>
@@ -2309,19 +2309,19 @@
         <v>0.0333333333333333</v>
       </c>
       <c r="L24">
-        <v>0.913978494623656</v>
+        <v>0.91156462585034</v>
       </c>
       <c r="M24">
-        <v>0.913978494623656</v>
+        <v>0.91156462585034</v>
       </c>
       <c r="N24">
-        <v>0.808409112789193</v>
+        <v>0.604606176882374</v>
       </c>
       <c r="O24">
-        <v>0.732759824454356</v>
+        <v>0.546411270524647</v>
       </c>
       <c r="P24">
-        <v>6.50645</v>
+        <v>8.47514</v>
       </c>
       <c r="Q24">
         <v>0.2697</v>
@@ -2347,52 +2347,52 @@
     </row>
     <row r="25" spans="1:23">
       <c r="A25" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B25">
-        <v>1210637</v>
+        <v>1893200</v>
       </c>
       <c r="C25">
-        <v>385.864507057036</v>
+        <v>330.68245485288</v>
       </c>
       <c r="D25">
-        <v>3426.30738301591</v>
+        <v>3800.91230425839</v>
       </c>
       <c r="E25">
-        <v>0.0748299285769463</v>
+        <v>0.296296298503876</v>
       </c>
       <c r="F25">
-        <v>3198.79125976562</v>
+        <v>2772.69604492188</v>
       </c>
       <c r="G25">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H25">
-        <v>0.204068381339312</v>
+        <v>0.343015007674694</v>
       </c>
       <c r="I25">
-        <v>0.204068381339312</v>
+        <v>0.343015007674694</v>
       </c>
       <c r="J25">
-        <v>0.0333333333333333</v>
+        <v>0.036904761798325</v>
       </c>
       <c r="K25">
         <v>0.0333333333333333</v>
       </c>
       <c r="L25">
-        <v>0.91156462585034</v>
+        <v>0.793650793650794</v>
       </c>
       <c r="M25">
-        <v>0.91156462585034</v>
+        <v>0.793650793650794</v>
       </c>
       <c r="N25">
-        <v>0.604606176882374</v>
+        <v>1.02849214203504</v>
       </c>
       <c r="O25">
-        <v>0.546411270524647</v>
+        <v>0.898341860583123</v>
       </c>
       <c r="P25">
-        <v>8.47514</v>
+        <v>26.6819</v>
       </c>
       <c r="Q25">
         <v>0.2697</v>
@@ -2418,52 +2418,52 @@
     </row>
     <row r="26" spans="1:23">
       <c r="A26" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B26">
-        <v>1893200</v>
+        <v>820850</v>
       </c>
       <c r="C26">
-        <v>334.465398242699</v>
+        <v>419.914801484173</v>
       </c>
       <c r="D26">
-        <v>3799.31948597213</v>
+        <v>4221.10856712928</v>
       </c>
       <c r="E26">
-        <v>0.296296298503876</v>
+        <v>0.184210523962975</v>
       </c>
       <c r="F26">
-        <v>2772.69604492188</v>
+        <v>3520.888671875</v>
       </c>
       <c r="G26">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H26">
-        <v>0.343015007674694</v>
+        <v>0.233447596430779</v>
       </c>
       <c r="I26">
-        <v>0.343015007674694</v>
+        <v>0.233447596430779</v>
       </c>
       <c r="J26">
-        <v>0.036904761798325</v>
+        <v>0.0333333333333333</v>
       </c>
       <c r="K26">
         <v>0.0333333333333333</v>
       </c>
       <c r="L26">
-        <v>0.793650793650794</v>
+        <v>0.912280701754386</v>
       </c>
       <c r="M26">
-        <v>0.793650793650794</v>
+        <v>0.912280701754386</v>
       </c>
       <c r="N26">
-        <v>1.02849214203504</v>
+        <v>0.728442311372076</v>
       </c>
       <c r="O26">
-        <v>0.898341860583123</v>
+        <v>0.648926950480232</v>
       </c>
       <c r="P26">
-        <v>26.6819</v>
+        <v>13.9209</v>
       </c>
       <c r="Q26">
         <v>0.2697</v>
@@ -2489,31 +2489,31 @@
     </row>
     <row r="27" spans="1:23">
       <c r="A27" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B27">
-        <v>820850</v>
+        <v>1941310</v>
       </c>
       <c r="C27">
-        <v>424.718545678186</v>
+        <v>406.172989180535</v>
       </c>
       <c r="D27">
-        <v>4220.02385071535</v>
+        <v>4084.79742801413</v>
       </c>
       <c r="E27">
-        <v>0.184210523962975</v>
+        <v>0.184615388512611</v>
       </c>
       <c r="F27">
-        <v>3520.888671875</v>
+        <v>3405.66674804688</v>
       </c>
       <c r="G27">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H27">
-        <v>0.233447596430779</v>
+        <v>0.175071448087692</v>
       </c>
       <c r="I27">
-        <v>0.233447596430779</v>
+        <v>0.175071448087692</v>
       </c>
       <c r="J27">
         <v>0.0333333333333333</v>
@@ -2522,19 +2522,19 @@
         <v>0.0333333333333333</v>
       </c>
       <c r="L27">
-        <v>0.912280701754386</v>
+        <v>0.897435897435897</v>
       </c>
       <c r="M27">
-        <v>0.912280701754386</v>
+        <v>0.897435897435897</v>
       </c>
       <c r="N27">
-        <v>0.728442311372076</v>
+        <v>0.962803890401003</v>
       </c>
       <c r="O27">
-        <v>0.648926950480232</v>
+        <v>0.857653886118404</v>
       </c>
       <c r="P27">
-        <v>13.9209</v>
+        <v>20.1754</v>
       </c>
       <c r="Q27">
         <v>0.2697</v>
@@ -2560,31 +2560,31 @@
     </row>
     <row r="28" spans="1:23">
       <c r="A28" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B28">
-        <v>1941310</v>
+        <v>966681</v>
       </c>
       <c r="C28">
-        <v>410.819529696956</v>
+        <v>343.296210327776</v>
       </c>
       <c r="D28">
-        <v>4083.74538107751</v>
+        <v>3714.80198804384</v>
       </c>
       <c r="E28">
-        <v>0.184615388512611</v>
+        <v>0.248062014579773</v>
       </c>
       <c r="F28">
-        <v>3405.66674804688</v>
+        <v>2878.45947265625</v>
       </c>
       <c r="G28">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H28">
-        <v>0.175071448087692</v>
+        <v>0.250944703817368</v>
       </c>
       <c r="I28">
-        <v>0.175071448087692</v>
+        <v>0.250944703817368</v>
       </c>
       <c r="J28">
         <v>0.0333333333333333</v>
@@ -2593,19 +2593,19 @@
         <v>0.0333333333333333</v>
       </c>
       <c r="L28">
-        <v>0.897435897435897</v>
+        <v>0.829457364341085</v>
       </c>
       <c r="M28">
-        <v>0.897435897435897</v>
+        <v>0.829457364341085</v>
       </c>
       <c r="N28">
-        <v>0.962803890401003</v>
+        <v>0.809131343510686</v>
       </c>
       <c r="O28">
-        <v>0.857653886118404</v>
+        <v>0.713308077419713</v>
       </c>
       <c r="P28">
-        <v>20.1754</v>
+        <v>6.98026</v>
       </c>
       <c r="Q28">
         <v>0.2697</v>
@@ -2631,52 +2631,52 @@
     </row>
     <row r="29" spans="1:23">
       <c r="A29" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B29">
-        <v>966681</v>
+        <v>3624888</v>
       </c>
       <c r="C29">
-        <v>347.223452643028</v>
+        <v>306.753656378754</v>
       </c>
       <c r="D29">
-        <v>3713.50640295657</v>
+        <v>3811.56501767503</v>
       </c>
       <c r="E29">
-        <v>0.248062014579773</v>
+        <v>0.353658527135849</v>
       </c>
       <c r="F29">
-        <v>2878.45947265625</v>
+        <v>2572.05859375</v>
       </c>
       <c r="G29">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H29">
-        <v>0.250944703817368</v>
+        <v>0.257421791553497</v>
       </c>
       <c r="I29">
-        <v>0.250944703817368</v>
+        <v>0.257421791553497</v>
       </c>
       <c r="J29">
-        <v>0.0333333333333333</v>
+        <v>0.0425287356723456</v>
       </c>
       <c r="K29">
         <v>0.0333333333333333</v>
       </c>
       <c r="L29">
-        <v>0.829457364341085</v>
+        <v>0.812244897959184</v>
       </c>
       <c r="M29">
-        <v>0.829457364341085</v>
+        <v>0.812244897959184</v>
       </c>
       <c r="N29">
-        <v>0.809131343510686</v>
+        <v>0.378737613686493</v>
       </c>
       <c r="O29">
-        <v>0.713308077419713</v>
+        <v>0.326556855627059</v>
       </c>
       <c r="P29">
-        <v>6.98026</v>
+        <v>8.13339</v>
       </c>
       <c r="Q29">
         <v>0.2697</v>
@@ -2702,52 +2702,52 @@
     </row>
     <row r="30" spans="1:23">
       <c r="A30" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B30">
-        <v>3624888</v>
+        <v>3100359</v>
       </c>
       <c r="C30">
-        <v>310.262858937496</v>
+        <v>298.208615710036</v>
       </c>
       <c r="D30">
-        <v>3809.64488805245</v>
+        <v>3265.24695842381</v>
       </c>
       <c r="E30">
-        <v>0.353658527135849</v>
+        <v>0.257777780294418</v>
       </c>
       <c r="F30">
-        <v>2572.05859375</v>
+        <v>2500.41040039062</v>
       </c>
       <c r="G30">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H30">
-        <v>0.257421791553497</v>
+        <v>0.303964786231518</v>
       </c>
       <c r="I30">
-        <v>0.257421791553497</v>
+        <v>0.303964786231518</v>
       </c>
       <c r="J30">
-        <v>0.0425287356723456</v>
+        <v>0.0367816092901957</v>
       </c>
       <c r="K30">
         <v>0.0333333333333333</v>
       </c>
       <c r="L30">
-        <v>0.812244897959184</v>
+        <v>0.799107142857143</v>
       </c>
       <c r="M30">
-        <v>0.812244897959184</v>
+        <v>0.799107142857143</v>
       </c>
       <c r="N30">
-        <v>0.378737613686493</v>
+        <v>0.338281144657913</v>
       </c>
       <c r="O30">
-        <v>0.326556855627059</v>
+        <v>0.297694999058287</v>
       </c>
       <c r="P30">
-        <v>8.13339</v>
+        <v>8.34776</v>
       </c>
       <c r="Q30">
         <v>0.2697</v>
@@ -2773,52 +2773,52 @@
     </row>
     <row r="31" spans="1:23">
       <c r="A31" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B31">
-        <v>3100359</v>
+        <v>1305396</v>
       </c>
       <c r="C31">
-        <v>301.620064654581</v>
+        <v>279.529698562008</v>
       </c>
       <c r="D31">
-        <v>3264.06214380473</v>
+        <v>3069.07330264624</v>
       </c>
       <c r="E31">
-        <v>0.257777780294418</v>
+        <v>0.259999990463257</v>
       </c>
       <c r="F31">
-        <v>2500.41040039062</v>
+        <v>2343.7919921875</v>
       </c>
       <c r="G31">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H31">
-        <v>0.303964786231518</v>
+        <v>0.346420831978321</v>
       </c>
       <c r="I31">
-        <v>0.303964786231518</v>
+        <v>0.346420831978321</v>
       </c>
       <c r="J31">
-        <v>0.0367816092901957</v>
+        <v>0.0384615388550085</v>
       </c>
       <c r="K31">
         <v>0.0333333333333333</v>
       </c>
       <c r="L31">
-        <v>0.799107142857143</v>
+        <v>0.893333333333333</v>
       </c>
       <c r="M31">
-        <v>0.799107142857143</v>
+        <v>0.893333333333333</v>
       </c>
       <c r="N31">
-        <v>0.338281144657913</v>
+        <v>0.503881556343059</v>
       </c>
       <c r="O31">
-        <v>0.297694999058287</v>
+        <v>0.443245533778378</v>
       </c>
       <c r="P31">
-        <v>8.34776</v>
+        <v>6.74015</v>
       </c>
       <c r="Q31">
         <v>0.2697</v>
@@ -2844,52 +2844,52 @@
     </row>
     <row r="32" spans="1:23">
       <c r="A32" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B32">
-        <v>1305396</v>
+        <v>900578</v>
       </c>
       <c r="C32">
-        <v>282.727464303477</v>
+        <v>306.965716620448</v>
       </c>
       <c r="D32">
-        <v>3067.94976338736</v>
+        <v>3470.04145664411</v>
       </c>
       <c r="E32">
-        <v>0.259999990463257</v>
+        <v>0.283333331346512</v>
       </c>
       <c r="F32">
-        <v>2343.7919921875</v>
+        <v>2573.83666992188</v>
       </c>
       <c r="G32">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H32">
-        <v>0.346420831978321</v>
+        <v>0.168648671358824</v>
       </c>
       <c r="I32">
-        <v>0.346420831978321</v>
+        <v>0.168648671358824</v>
       </c>
       <c r="J32">
-        <v>0.0384615388550085</v>
+        <v>0.0333333333333333</v>
       </c>
       <c r="K32">
         <v>0.0333333333333333</v>
       </c>
       <c r="L32">
-        <v>0.893333333333333</v>
+        <v>0.808333333333333</v>
       </c>
       <c r="M32">
-        <v>0.893333333333333</v>
+        <v>0.808333333333333</v>
       </c>
       <c r="N32">
-        <v>0.503881556343059</v>
+        <v>0.412355464660392</v>
       </c>
       <c r="O32">
-        <v>0.443245533778378</v>
+        <v>0.361117895554503</v>
       </c>
       <c r="P32">
-        <v>6.74015</v>
+        <v>7.10385</v>
       </c>
       <c r="Q32">
         <v>0.2697</v>
@@ -2915,31 +2915,31 @@
     </row>
     <row r="33" spans="1:23">
       <c r="A33" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B33">
-        <v>900578</v>
+        <v>639805</v>
       </c>
       <c r="C33">
-        <v>310.477345107382</v>
+        <v>307.594880111116</v>
       </c>
       <c r="D33">
-        <v>3468.65313841868</v>
+        <v>3714.87070153712</v>
       </c>
       <c r="E33">
-        <v>0.283333331346512</v>
+        <v>0.333333343267441</v>
       </c>
       <c r="F33">
-        <v>2573.83666992188</v>
+        <v>2579.11206054688</v>
       </c>
       <c r="G33">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H33">
-        <v>0.168648671358824</v>
+        <v>0.188250351697206</v>
       </c>
       <c r="I33">
-        <v>0.168648671358824</v>
+        <v>0.188250351697206</v>
       </c>
       <c r="J33">
         <v>0.0333333333333333</v>
@@ -2948,19 +2948,19 @@
         <v>0.0333333333333333</v>
       </c>
       <c r="L33">
-        <v>0.808333333333333</v>
+        <v>0.87</v>
       </c>
       <c r="M33">
-        <v>0.808333333333333</v>
+        <v>0.87</v>
       </c>
       <c r="N33">
-        <v>0.412355464660392</v>
+        <v>0.324086445089506</v>
       </c>
       <c r="O33">
-        <v>0.361117895554503</v>
+        <v>0.280796593022832</v>
       </c>
       <c r="P33">
-        <v>7.10385</v>
+        <v>6.50645</v>
       </c>
       <c r="Q33">
         <v>0.2697</v>
@@ -2986,31 +2986,31 @@
     </row>
     <row r="34" spans="1:23">
       <c r="A34" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B34">
-        <v>639805</v>
+        <v>1157792</v>
       </c>
       <c r="C34">
-        <v>311.113706106817</v>
+        <v>400.108322499043</v>
       </c>
       <c r="D34">
-        <v>3713.11128846062</v>
+        <v>3868.67811297963</v>
       </c>
       <c r="E34">
-        <v>0.333333343267441</v>
+        <v>0.148148149251938</v>
       </c>
       <c r="F34">
-        <v>2579.11206054688</v>
+        <v>3354.81591796875</v>
       </c>
       <c r="G34">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H34">
-        <v>0.188250351697206</v>
+        <v>0.221995271742344</v>
       </c>
       <c r="I34">
-        <v>0.188250351697206</v>
+        <v>0.221995271742344</v>
       </c>
       <c r="J34">
         <v>0.0333333333333333</v>
@@ -3019,19 +3019,19 @@
         <v>0.0333333333333333</v>
       </c>
       <c r="L34">
-        <v>0.87</v>
+        <v>0.911111111111111</v>
       </c>
       <c r="M34">
-        <v>0.87</v>
+        <v>0.911111111111111</v>
       </c>
       <c r="N34">
-        <v>0.324086445089506</v>
+        <v>0.379809934594193</v>
       </c>
       <c r="O34">
-        <v>0.280796593022832</v>
+        <v>0.340105755779062</v>
       </c>
       <c r="P34">
-        <v>6.50645</v>
+        <v>52.6529</v>
       </c>
       <c r="Q34">
         <v>0.2697</v>
@@ -3057,31 +3057,31 @@
     </row>
     <row r="35" spans="1:23">
       <c r="A35" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B35">
-        <v>1157792</v>
+        <v>940188</v>
       </c>
       <c r="C35">
-        <v>404.685484400429</v>
+        <v>563.004771660551</v>
       </c>
       <c r="D35">
-        <v>3867.88208481591</v>
+        <v>4864.03264222519</v>
       </c>
       <c r="E35">
-        <v>0.148148149251938</v>
+        <v>0.0333333350718021</v>
       </c>
       <c r="F35">
-        <v>3354.81591796875</v>
+        <v>4720.6650390625</v>
       </c>
       <c r="G35">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H35">
-        <v>0.221995271742344</v>
+        <v>0.232459001243114</v>
       </c>
       <c r="I35">
-        <v>0.221995271742344</v>
+        <v>0.232459001243114</v>
       </c>
       <c r="J35">
         <v>0.0333333333333333</v>
@@ -3090,19 +3090,19 @@
         <v>0.0333333333333333</v>
       </c>
       <c r="L35">
-        <v>0.911111111111111</v>
+        <v>0.975</v>
       </c>
       <c r="M35">
-        <v>0.911111111111111</v>
+        <v>0.975</v>
       </c>
       <c r="N35">
-        <v>0.379809934594193</v>
+        <v>0.22174431366884</v>
       </c>
       <c r="O35">
-        <v>0.340105755779062</v>
+        <v>0.201317072397537</v>
       </c>
       <c r="P35">
-        <v>52.6529</v>
+        <v>6.50645</v>
       </c>
       <c r="Q35">
         <v>0.2697</v>
@@ -3128,31 +3128,31 @@
     </row>
     <row r="36" spans="1:23">
       <c r="A36" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B36">
-        <v>940188</v>
+        <v>1515708</v>
       </c>
       <c r="C36">
-        <v>569.445437465869</v>
+        <v>324.485305114995</v>
       </c>
       <c r="D36">
-        <v>4863.81055028889</v>
+        <v>3788.15441334468</v>
       </c>
       <c r="E36">
-        <v>0.0333333350718021</v>
+        <v>0.308176100254059</v>
       </c>
       <c r="F36">
-        <v>4720.6650390625</v>
+        <v>2720.734375</v>
       </c>
       <c r="G36">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H36">
-        <v>0.232459001243114</v>
+        <v>0.224189573898911</v>
       </c>
       <c r="I36">
-        <v>0.232459001243114</v>
+        <v>0.224189573898911</v>
       </c>
       <c r="J36">
         <v>0.0333333333333333</v>
@@ -3161,19 +3161,19 @@
         <v>0.0333333333333333</v>
       </c>
       <c r="L36">
-        <v>0.975</v>
+        <v>0.779874213836478</v>
       </c>
       <c r="M36">
-        <v>0.975</v>
+        <v>0.779874213836478</v>
       </c>
       <c r="N36">
-        <v>0.22174431366884</v>
+        <v>0.296166515551051</v>
       </c>
       <c r="O36">
-        <v>0.201317072397537</v>
+        <v>0.258044630816374</v>
       </c>
       <c r="P36">
-        <v>6.50645</v>
+        <v>7.36177</v>
       </c>
       <c r="Q36">
         <v>0.2697</v>
@@ -3199,31 +3199,31 @@
     </row>
     <row r="37" spans="1:23">
       <c r="A37" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B37">
-        <v>1515708</v>
+        <v>1292018</v>
       </c>
       <c r="C37">
-        <v>328.197354309212</v>
+        <v>311.607078518952</v>
       </c>
       <c r="D37">
-        <v>3786.50086416107</v>
+        <v>3728.46070012223</v>
       </c>
       <c r="E37">
-        <v>0.308176100254059</v>
+        <v>0.326530605554581</v>
       </c>
       <c r="F37">
-        <v>2720.734375</v>
+        <v>2612.75341796875</v>
       </c>
       <c r="G37">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H37">
-        <v>0.224189573898911</v>
+        <v>0.140036443248391</v>
       </c>
       <c r="I37">
-        <v>0.224189573898911</v>
+        <v>0.140036443248391</v>
       </c>
       <c r="J37">
         <v>0.0333333333333333</v>
@@ -3232,19 +3232,19 @@
         <v>0.0333333333333333</v>
       </c>
       <c r="L37">
-        <v>0.779874213836478</v>
+        <v>0.855172413793103</v>
       </c>
       <c r="M37">
-        <v>0.779874213836478</v>
+        <v>0.855172413793103</v>
       </c>
       <c r="N37">
-        <v>0.296166515551051</v>
+        <v>0.289182869013475</v>
       </c>
       <c r="O37">
-        <v>0.258044630816374</v>
+        <v>0.250945441468711</v>
       </c>
       <c r="P37">
-        <v>7.36177</v>
+        <v>11.072</v>
       </c>
       <c r="Q37">
         <v>0.2697</v>
@@ -3270,31 +3270,31 @@
     </row>
     <row r="38" spans="1:23">
       <c r="A38" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B38">
-        <v>1292018</v>
+        <v>1579651</v>
       </c>
       <c r="C38">
-        <v>315.171803289211</v>
+        <v>419.1117794595</v>
       </c>
       <c r="D38">
-        <v>3726.73234877105</v>
+        <v>3877.02270308955</v>
       </c>
       <c r="E38">
-        <v>0.326530605554581</v>
+        <v>0.104938268661499</v>
       </c>
       <c r="F38">
-        <v>2612.75341796875</v>
+        <v>3514.15551757812</v>
       </c>
       <c r="G38">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H38">
-        <v>0.140036443248391</v>
+        <v>0.173469252884388</v>
       </c>
       <c r="I38">
-        <v>0.140036443248391</v>
+        <v>0.173469252884388</v>
       </c>
       <c r="J38">
         <v>0.0333333333333333</v>
@@ -3303,19 +3303,19 @@
         <v>0.0333333333333333</v>
       </c>
       <c r="L38">
-        <v>0.855172413793103</v>
+        <v>0.827160493827161</v>
       </c>
       <c r="M38">
-        <v>0.855172413793103</v>
+        <v>0.827160493827161</v>
       </c>
       <c r="N38">
-        <v>0.289182869013475</v>
+        <v>0.340798450459023</v>
       </c>
       <c r="O38">
-        <v>0.250945441468711</v>
+        <v>0.306892291678384</v>
       </c>
       <c r="P38">
-        <v>11.072</v>
+        <v>10.8682</v>
       </c>
       <c r="Q38">
         <v>0.2697</v>
@@ -3341,31 +3341,31 @@
     </row>
     <row r="39" spans="1:23">
       <c r="A39" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B39">
-        <v>1579651</v>
+        <v>907294</v>
       </c>
       <c r="C39">
-        <v>423.90633723671</v>
+        <v>386.569456767506</v>
       </c>
       <c r="D39">
-        <v>3876.46058254018</v>
+        <v>4288.02865927875</v>
       </c>
       <c r="E39">
-        <v>0.104938268661499</v>
+        <v>0.26829269528389</v>
       </c>
       <c r="F39">
-        <v>3514.15551757812</v>
+        <v>3241.29565429688</v>
       </c>
       <c r="G39">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H39">
-        <v>0.173469252884388</v>
+        <v>0.180655494332314</v>
       </c>
       <c r="I39">
-        <v>0.173469252884388</v>
+        <v>0.180655494332314</v>
       </c>
       <c r="J39">
         <v>0.0333333333333333</v>
@@ -3374,19 +3374,19 @@
         <v>0.0333333333333333</v>
       </c>
       <c r="L39">
-        <v>0.827160493827161</v>
+        <v>0.910569105691057</v>
       </c>
       <c r="M39">
-        <v>0.827160493827161</v>
+        <v>0.910569105691057</v>
       </c>
       <c r="N39">
-        <v>0.340798450459023</v>
+        <v>0.212847194109036</v>
       </c>
       <c r="O39">
-        <v>0.306892291678384</v>
+        <v>0.186943332699227</v>
       </c>
       <c r="P39">
-        <v>10.8682</v>
+        <v>7.05335</v>
       </c>
       <c r="Q39">
         <v>0.2697</v>
@@ -3412,31 +3412,31 @@
     </row>
     <row r="40" spans="1:23">
       <c r="A40" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B40">
-        <v>907294</v>
+        <v>1219332</v>
       </c>
       <c r="C40">
-        <v>390.991736660871</v>
+        <v>466.269487346979</v>
       </c>
       <c r="D40">
-        <v>4286.40715654912</v>
+        <v>4267.66443380025</v>
       </c>
       <c r="E40">
-        <v>0.26829269528389</v>
+        <v>0.0942028984427452</v>
       </c>
       <c r="F40">
-        <v>3241.29565429688</v>
+        <v>3909.56201171875</v>
       </c>
       <c r="G40">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H40">
-        <v>0.180655494332314</v>
+        <v>0.169438641518354</v>
       </c>
       <c r="I40">
-        <v>0.180655494332314</v>
+        <v>0.169438641518354</v>
       </c>
       <c r="J40">
         <v>0.0333333333333333</v>
@@ -3445,19 +3445,19 @@
         <v>0.0333333333333333</v>
       </c>
       <c r="L40">
-        <v>0.910569105691057</v>
+        <v>0.898550724637681</v>
       </c>
       <c r="M40">
-        <v>0.910569105691057</v>
+        <v>0.898550724637681</v>
       </c>
       <c r="N40">
-        <v>0.212847194109036</v>
+        <v>0.318387934772336</v>
       </c>
       <c r="O40">
-        <v>0.186943332699227</v>
+        <v>0.287086831575739</v>
       </c>
       <c r="P40">
-        <v>7.05335</v>
+        <v>6.90841</v>
       </c>
       <c r="Q40">
         <v>0.2697</v>
@@ -3483,31 +3483,31 @@
     </row>
     <row r="41" spans="1:23">
       <c r="A41" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B41">
-        <v>1219332</v>
+        <v>600099</v>
       </c>
       <c r="C41">
-        <v>471.603520190718</v>
+        <v>355.444877481846</v>
       </c>
       <c r="D41">
-        <v>4267.10969438521</v>
+        <v>3702.16480120881</v>
       </c>
       <c r="E41">
-        <v>0.0942028984427452</v>
+        <v>0.215686276555061</v>
       </c>
       <c r="F41">
-        <v>3909.56201171875</v>
+        <v>2980.3232421875</v>
       </c>
       <c r="G41">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H41">
-        <v>0.169438641518354</v>
+        <v>0.190052464604378</v>
       </c>
       <c r="I41">
-        <v>0.169438641518354</v>
+        <v>0.190052464604378</v>
       </c>
       <c r="J41">
         <v>0.0333333333333333</v>
@@ -3516,19 +3516,19 @@
         <v>0.0333333333333333</v>
       </c>
       <c r="L41">
-        <v>0.898550724637681</v>
+        <v>0.911764705882353</v>
       </c>
       <c r="M41">
-        <v>0.898550724637681</v>
+        <v>0.911764705882353</v>
       </c>
       <c r="N41">
-        <v>0.318387934772336</v>
+        <v>0.397462776668218</v>
       </c>
       <c r="O41">
-        <v>0.287086831575739</v>
+        <v>0.352335345005512</v>
       </c>
       <c r="P41">
-        <v>6.90841</v>
+        <v>11.3219</v>
       </c>
       <c r="Q41">
         <v>0.2697</v>
@@ -3554,31 +3554,31 @@
     </row>
     <row r="42" spans="1:23">
       <c r="A42" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B42">
-        <v>600099</v>
+        <v>1226361</v>
       </c>
       <c r="C42">
-        <v>359.511098202003</v>
+        <v>398.606692568429</v>
       </c>
       <c r="D42">
-        <v>3701.04659049724</v>
+        <v>3795.08949492213</v>
       </c>
       <c r="E42">
-        <v>0.215686276555061</v>
+        <v>0.133333340287209</v>
       </c>
       <c r="F42">
-        <v>2980.3232421875</v>
+        <v>3342.22509765625</v>
       </c>
       <c r="G42">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H42">
-        <v>0.190052464604378</v>
+        <v>0.180553380399942</v>
       </c>
       <c r="I42">
-        <v>0.190052464604378</v>
+        <v>0.180553380399942</v>
       </c>
       <c r="J42">
         <v>0.0333333333333333</v>
@@ -3587,19 +3587,19 @@
         <v>0.0333333333333333</v>
       </c>
       <c r="L42">
-        <v>0.911764705882353</v>
+        <v>0.903703703703704</v>
       </c>
       <c r="M42">
-        <v>0.911764705882353</v>
+        <v>0.903703703703704</v>
       </c>
       <c r="N42">
-        <v>0.397462776668218</v>
+        <v>0.441782571545669</v>
       </c>
       <c r="O42">
-        <v>0.352335345005512</v>
+        <v>0.396389407216804</v>
       </c>
       <c r="P42">
-        <v>11.3219</v>
+        <v>8.95148</v>
       </c>
       <c r="Q42">
         <v>0.2697</v>
@@ -3625,31 +3625,31 @@
     </row>
     <row r="43" spans="1:23">
       <c r="A43" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B43">
-        <v>1226361</v>
+        <v>459231</v>
       </c>
       <c r="C43">
-        <v>403.16667611355</v>
+        <v>378.175213845833</v>
       </c>
       <c r="D43">
-        <v>3794.38795894989</v>
+        <v>6439.0079159015</v>
       </c>
       <c r="E43">
-        <v>0.133333340287209</v>
+        <v>0.539215683937073</v>
       </c>
       <c r="F43">
-        <v>3342.22509765625</v>
+        <v>3170.91186523438</v>
       </c>
       <c r="G43">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H43">
-        <v>0.180553380399942</v>
+        <v>0.0944860577583313</v>
       </c>
       <c r="I43">
-        <v>0.180553380399942</v>
+        <v>0.0944860577583313</v>
       </c>
       <c r="J43">
         <v>0.0333333333333333</v>
@@ -3658,19 +3658,19 @@
         <v>0.0333333333333333</v>
       </c>
       <c r="L43">
-        <v>0.903703703703704</v>
+        <v>0.653061224489796</v>
       </c>
       <c r="M43">
-        <v>0.903703703703704</v>
+        <v>0.653061224489796</v>
       </c>
       <c r="N43">
-        <v>0.441782571545669</v>
+        <v>0.241445024661264</v>
       </c>
       <c r="O43">
-        <v>0.396389407216804</v>
+        <v>0.194783971016635</v>
       </c>
       <c r="P43">
-        <v>8.95148</v>
+        <v>7.25033</v>
       </c>
       <c r="Q43">
         <v>0.2697</v>
@@ -3696,31 +3696,31 @@
     </row>
     <row r="44" spans="1:23">
       <c r="A44" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B44">
-        <v>459231</v>
+        <v>1365857</v>
       </c>
       <c r="C44">
-        <v>382.501465222091</v>
+        <v>395.06068893332</v>
       </c>
       <c r="D44">
-        <v>6433.94528135989</v>
+        <v>5411.62056693397</v>
       </c>
       <c r="E44">
-        <v>0.539215683937073</v>
+        <v>0.418439716100693</v>
       </c>
       <c r="F44">
-        <v>3170.91186523438</v>
+        <v>3312.49267578125</v>
       </c>
       <c r="G44">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H44">
-        <v>0.0944860577583313</v>
+        <v>0.0894328560680151</v>
       </c>
       <c r="I44">
-        <v>0.0944860577583313</v>
+        <v>0.0894328560680151</v>
       </c>
       <c r="J44">
         <v>0.0333333333333333</v>
@@ -3729,19 +3729,19 @@
         <v>0.0333333333333333</v>
       </c>
       <c r="L44">
-        <v>0.653061224489796</v>
+        <v>0.77536231884058</v>
       </c>
       <c r="M44">
-        <v>0.653061224489796</v>
+        <v>0.77536231884058</v>
       </c>
       <c r="N44">
-        <v>0.241445024661264</v>
+        <v>0.187896798821736</v>
       </c>
       <c r="O44">
-        <v>0.194783971016635</v>
+        <v>0.159125556794229</v>
       </c>
       <c r="P44">
-        <v>7.25033</v>
+        <v>6.84467</v>
       </c>
       <c r="Q44">
         <v>0.2697</v>
@@ -3767,52 +3767,52 @@
     </row>
     <row r="45" spans="1:23">
       <c r="A45" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B45">
-        <v>1365857</v>
+        <v>1844428</v>
       </c>
       <c r="C45">
-        <v>399.580106882006</v>
+        <v>389.057663269495</v>
       </c>
       <c r="D45">
-        <v>5408.36879060786</v>
+        <v>4861.33747376769</v>
       </c>
       <c r="E45">
-        <v>0.418439716100693</v>
+        <v>0.357575744390488</v>
       </c>
       <c r="F45">
-        <v>3312.49267578125</v>
+        <v>3262.15869140625</v>
       </c>
       <c r="G45">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H45">
-        <v>0.0894328560680151</v>
+        <v>0.080965381115675</v>
       </c>
       <c r="I45">
-        <v>0.0894328560680151</v>
+        <v>0.080965381115675</v>
       </c>
       <c r="J45">
-        <v>0.0333333333333333</v>
+        <v>0.0367231639668047</v>
       </c>
       <c r="K45">
         <v>0.0333333333333333</v>
       </c>
       <c r="L45">
-        <v>0.77536231884058</v>
+        <v>0.920731707317073</v>
       </c>
       <c r="M45">
-        <v>0.77536231884058</v>
+        <v>0.920731707317073</v>
       </c>
       <c r="N45">
-        <v>0.187896798821736</v>
+        <v>0.205582749135032</v>
       </c>
       <c r="O45">
-        <v>0.159125556794229</v>
+        <v>0.177085777606333</v>
       </c>
       <c r="P45">
-        <v>6.84467</v>
+        <v>6.52538</v>
       </c>
       <c r="Q45">
         <v>0.2697</v>
@@ -3838,52 +3838,52 @@
     </row>
     <row r="46" spans="1:23">
       <c r="A46" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B46">
-        <v>1844428</v>
+        <v>524936</v>
       </c>
       <c r="C46">
-        <v>393.508407764478</v>
+        <v>339.523005530242</v>
       </c>
       <c r="D46">
-        <v>4858.86017272872</v>
+        <v>4532.05582727231</v>
       </c>
       <c r="E46">
-        <v>0.357575744390488</v>
+        <v>0.401960790157318</v>
       </c>
       <c r="F46">
-        <v>3262.15869140625</v>
+        <v>2846.82202148438</v>
       </c>
       <c r="G46">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H46">
-        <v>0.080965381115675</v>
+        <v>0.0791360074654222</v>
       </c>
       <c r="I46">
-        <v>0.080965381115675</v>
+        <v>0.0791360074654222</v>
       </c>
       <c r="J46">
-        <v>0.0367231639668047</v>
+        <v>0.0382113821292231</v>
       </c>
       <c r="K46">
         <v>0.0333333333333333</v>
       </c>
       <c r="L46">
-        <v>0.920731707317073</v>
+        <v>0.92156862745098</v>
       </c>
       <c r="M46">
-        <v>0.920731707317073</v>
+        <v>0.92156862745098</v>
       </c>
       <c r="N46">
-        <v>0.205582749135032</v>
+        <v>0.164870051124266</v>
       </c>
       <c r="O46">
-        <v>0.177085777606333</v>
+        <v>0.140320357151839</v>
       </c>
       <c r="P46">
-        <v>6.52538</v>
+        <v>6.50645</v>
       </c>
       <c r="Q46">
         <v>0.2697</v>
@@ -3909,52 +3909,52 @@
     </row>
     <row r="47" spans="1:23">
       <c r="A47" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B47">
-        <v>524936</v>
+        <v>1265612</v>
       </c>
       <c r="C47">
-        <v>343.407083111659</v>
+        <v>419.528213013903</v>
       </c>
       <c r="D47">
-        <v>4529.44521768691</v>
+        <v>4319.83872172958</v>
       </c>
       <c r="E47">
-        <v>0.401960790157318</v>
+        <v>0.20567375421524</v>
       </c>
       <c r="F47">
-        <v>2846.82202148438</v>
+        <v>3517.64721679688</v>
       </c>
       <c r="G47">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H47">
-        <v>0.0791360074654222</v>
+        <v>0.0895548108965158</v>
       </c>
       <c r="I47">
-        <v>0.0791360074654222</v>
+        <v>0.0895548108965158</v>
       </c>
       <c r="J47">
-        <v>0.0382113821292231</v>
+        <v>0.0333333333333333</v>
       </c>
       <c r="K47">
         <v>0.0333333333333333</v>
       </c>
       <c r="L47">
-        <v>0.92156862745098</v>
+        <v>0.907801418439716</v>
       </c>
       <c r="M47">
-        <v>0.92156862745098</v>
+        <v>0.907801418439716</v>
       </c>
       <c r="N47">
-        <v>0.164870051124266</v>
+        <v>0.217921555227771</v>
       </c>
       <c r="O47">
-        <v>0.140320357151839</v>
+        <v>0.193490892610636</v>
       </c>
       <c r="P47">
-        <v>6.50645</v>
+        <v>6.66102</v>
       </c>
       <c r="Q47">
         <v>0.2697</v>
@@ -3980,52 +3980,52 @@
     </row>
     <row r="48" spans="1:23">
       <c r="A48" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B48">
-        <v>1265612</v>
+        <v>927893</v>
       </c>
       <c r="C48">
-        <v>424.327534710512</v>
+        <v>444.514109809422</v>
       </c>
       <c r="D48">
-        <v>4318.59604025422</v>
+        <v>4268.94216388794</v>
       </c>
       <c r="E48">
-        <v>0.20567375421524</v>
+        <v>0.141666665673256</v>
       </c>
       <c r="F48">
-        <v>3517.64721679688</v>
+        <v>3727.14819335938</v>
       </c>
       <c r="G48">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H48">
-        <v>0.0895548108965158</v>
+        <v>0.0882572550326586</v>
       </c>
       <c r="I48">
-        <v>0.0895548108965158</v>
+        <v>0.0882572550326586</v>
       </c>
       <c r="J48">
-        <v>0.0333333333333333</v>
+        <v>0.0568627470599396</v>
       </c>
       <c r="K48">
         <v>0.0333333333333333</v>
       </c>
       <c r="L48">
-        <v>0.907801418439716</v>
+        <v>0.891666666666667</v>
       </c>
       <c r="M48">
-        <v>0.907801418439716</v>
+        <v>0.891666666666667</v>
       </c>
       <c r="N48">
-        <v>0.217921555227771</v>
+        <v>0.190001969203657</v>
       </c>
       <c r="O48">
-        <v>0.193490892610636</v>
+        <v>0.170289724033775</v>
       </c>
       <c r="P48">
-        <v>6.66102</v>
+        <v>6.50645</v>
       </c>
       <c r="Q48">
         <v>0.2697</v>
@@ -4051,52 +4051,52 @@
     </row>
     <row r="49" spans="1:23">
       <c r="A49" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B49">
-        <v>927893</v>
+        <v>1147528</v>
       </c>
       <c r="C49">
-        <v>449.599265337655</v>
+        <v>414.842156282089</v>
       </c>
       <c r="D49">
-        <v>4268.10286638042</v>
+        <v>4469.49245357042</v>
       </c>
       <c r="E49">
-        <v>0.141666665673256</v>
+        <v>0.244444444775581</v>
       </c>
       <c r="F49">
-        <v>3727.14819335938</v>
+        <v>3478.35571289062</v>
       </c>
       <c r="G49">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H49">
-        <v>0.0882572550326586</v>
+        <v>0.144833575934172</v>
       </c>
       <c r="I49">
-        <v>0.0882572550326586</v>
+        <v>0.144833575934172</v>
       </c>
       <c r="J49">
-        <v>0.0568627470599396</v>
+        <v>0.0393939393518631</v>
       </c>
       <c r="K49">
         <v>0.0333333333333333</v>
       </c>
       <c r="L49">
-        <v>0.891666666666667</v>
+        <v>0.903703703703704</v>
       </c>
       <c r="M49">
-        <v>0.891666666666667</v>
+        <v>0.903703703703704</v>
       </c>
       <c r="N49">
-        <v>0.190001969203657</v>
+        <v>0.259545367773698</v>
       </c>
       <c r="O49">
-        <v>0.170289724033775</v>
+        <v>0.22895527118449</v>
       </c>
       <c r="P49">
-        <v>6.50645</v>
+        <v>8.35565</v>
       </c>
       <c r="Q49">
         <v>0.2697</v>
@@ -4122,52 +4122,52 @@
     </row>
     <row r="50" spans="1:23">
       <c r="A50" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B50">
-        <v>1147528</v>
+        <v>1569189</v>
       </c>
       <c r="C50">
-        <v>419.587870395115</v>
+        <v>719.8259263789</v>
       </c>
       <c r="D50">
-        <v>4467.95707547227</v>
+        <v>6222.09170305245</v>
       </c>
       <c r="E50">
-        <v>0.244444444775581</v>
+        <v>0.0338983051478863</v>
       </c>
       <c r="F50">
-        <v>3478.35571289062</v>
+        <v>6035.57421875</v>
       </c>
       <c r="G50">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H50">
-        <v>0.144833575934172</v>
+        <v>0.0944770984351635</v>
       </c>
       <c r="I50">
-        <v>0.144833575934172</v>
+        <v>0.0944770984351635</v>
       </c>
       <c r="J50">
-        <v>0.0393939393518631</v>
+        <v>0.0666666663562259</v>
       </c>
       <c r="K50">
         <v>0.0333333333333333</v>
       </c>
       <c r="L50">
-        <v>0.903703703703704</v>
+        <v>0.92090395480226</v>
       </c>
       <c r="M50">
-        <v>0.903703703703704</v>
+        <v>0.92090395480226</v>
       </c>
       <c r="N50">
-        <v>0.259545367773698</v>
+        <v>0.187103869577452</v>
       </c>
       <c r="O50">
-        <v>0.22895527118449</v>
+        <v>0.169857650660892</v>
       </c>
       <c r="P50">
-        <v>8.35565</v>
+        <v>7.41996</v>
       </c>
       <c r="Q50">
         <v>0.2697</v>
@@ -4193,52 +4193,52 @@
     </row>
     <row r="51" spans="1:23">
       <c r="A51" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B51">
-        <v>1569189</v>
+        <v>2647668</v>
       </c>
       <c r="C51">
-        <v>728.060595893577</v>
+        <v>538.447887030502</v>
       </c>
       <c r="D51">
-        <v>6221.80276727945</v>
+        <v>5036.24495862826</v>
       </c>
       <c r="E51">
-        <v>0.0338983051478863</v>
+        <v>0.115942031145096</v>
       </c>
       <c r="F51">
-        <v>6035.57421875</v>
+        <v>4514.76123046875</v>
       </c>
       <c r="G51">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H51">
-        <v>0.0944770984351635</v>
+        <v>0.212708599865437</v>
       </c>
       <c r="I51">
-        <v>0.0944770984351635</v>
+        <v>0.212708599865437</v>
       </c>
       <c r="J51">
-        <v>0.0666666663562259</v>
+        <v>0.0499999990764385</v>
       </c>
       <c r="K51">
         <v>0.0333333333333333</v>
       </c>
       <c r="L51">
-        <v>0.92090395480226</v>
+        <v>0.922705314009662</v>
       </c>
       <c r="M51">
-        <v>0.92090395480226</v>
+        <v>0.922705314009662</v>
       </c>
       <c r="N51">
-        <v>0.187103869577452</v>
+        <v>0.230242842089157</v>
       </c>
       <c r="O51">
-        <v>0.169857650660892</v>
+        <v>0.207050780085804</v>
       </c>
       <c r="P51">
-        <v>7.41996</v>
+        <v>7.16257</v>
       </c>
       <c r="Q51">
         <v>0.2697</v>
@@ -4264,52 +4264,52 @@
     </row>
     <row r="52" spans="1:23">
       <c r="A52" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B52">
-        <v>2647668</v>
+        <v>1038345</v>
       </c>
       <c r="C52">
-        <v>544.607626820477</v>
+        <v>627.487623679808</v>
       </c>
       <c r="D52">
-        <v>5035.43712388468</v>
+        <v>5560.29702141439</v>
       </c>
       <c r="E52">
-        <v>0.115942031145096</v>
+        <v>0.060606062412262</v>
       </c>
       <c r="F52">
-        <v>4514.76123046875</v>
+        <v>5261.3388671875</v>
       </c>
       <c r="G52">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H52">
-        <v>0.212708599865437</v>
+        <v>0.106365650892258</v>
       </c>
       <c r="I52">
-        <v>0.212708599865437</v>
+        <v>0.106365650892258</v>
       </c>
       <c r="J52">
-        <v>0.0499999990764385</v>
+        <v>0.0333333333333333</v>
       </c>
       <c r="K52">
         <v>0.0333333333333333</v>
       </c>
       <c r="L52">
-        <v>0.922705314009662</v>
+        <v>0.878787878787879</v>
       </c>
       <c r="M52">
-        <v>0.922705314009662</v>
+        <v>0.878787878787879</v>
       </c>
       <c r="N52">
-        <v>0.230242842089157</v>
+        <v>0.20378248862466</v>
       </c>
       <c r="O52">
-        <v>0.207050780085804</v>
+        <v>0.184464892693749</v>
       </c>
       <c r="P52">
-        <v>7.16257</v>
+        <v>6.50645</v>
       </c>
       <c r="Q52">
         <v>0.2697</v>
@@ -4335,52 +4335,52 @@
     </row>
     <row r="53" spans="1:23">
       <c r="A53" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B53">
-        <v>1038345</v>
+        <v>7645628</v>
       </c>
       <c r="C53">
-        <v>634.665960853</v>
+        <v>745.589134751005</v>
       </c>
       <c r="D53">
-        <v>5559.8339028724</v>
+        <v>6413.05916038537</v>
       </c>
       <c r="E53">
-        <v>0.060606062412262</v>
+        <v>0.0284900292754173</v>
       </c>
       <c r="F53">
-        <v>5261.3388671875</v>
+        <v>6251.5927734375</v>
       </c>
       <c r="G53">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H53">
-        <v>0.106365650892258</v>
+        <v>0.212258517742157</v>
       </c>
       <c r="I53">
-        <v>0.106365650892258</v>
+        <v>0.212258517742157</v>
       </c>
       <c r="J53">
-        <v>0.0333333333333333</v>
+        <v>0.0533333330241342</v>
       </c>
       <c r="K53">
         <v>0.0333333333333333</v>
       </c>
       <c r="L53">
-        <v>0.878787878787879</v>
+        <v>0.937321937321937</v>
       </c>
       <c r="M53">
-        <v>0.878787878787879</v>
+        <v>0.937321937321937</v>
       </c>
       <c r="N53">
-        <v>0.20378248862466</v>
+        <v>0.271891992907135</v>
       </c>
       <c r="O53">
-        <v>0.184464892693749</v>
+        <v>0.246969979520418</v>
       </c>
       <c r="P53">
-        <v>6.50645</v>
+        <v>8.37511</v>
       </c>
       <c r="Q53">
         <v>0.2697</v>
@@ -4406,52 +4406,52 @@
     </row>
     <row r="54" spans="1:23">
       <c r="A54" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B54">
-        <v>7645628</v>
+        <v>1521494</v>
       </c>
       <c r="C54">
-        <v>754.118530391551</v>
+        <v>441.441813173094</v>
       </c>
       <c r="D54">
-        <v>6412.80903147386</v>
+        <v>4163.61882806161</v>
       </c>
       <c r="E54">
-        <v>0.0284900292754173</v>
+        <v>0.124183006584644</v>
       </c>
       <c r="F54">
-        <v>6251.5927734375</v>
+        <v>3701.3876953125</v>
       </c>
       <c r="G54">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H54">
-        <v>0.212258517742157</v>
+        <v>0.118592367041856</v>
       </c>
       <c r="I54">
-        <v>0.212258517742157</v>
+        <v>0.118592367041856</v>
       </c>
       <c r="J54">
-        <v>0.0533333330241342</v>
+        <v>0.117543860287633</v>
       </c>
       <c r="K54">
         <v>0.0333333333333333</v>
       </c>
       <c r="L54">
-        <v>0.937321937321937</v>
+        <v>0.934640522875817</v>
       </c>
       <c r="M54">
-        <v>0.937321937321937</v>
+        <v>0.934640522875817</v>
       </c>
       <c r="N54">
-        <v>0.271891992907135</v>
+        <v>0.597967909477195</v>
       </c>
       <c r="O54">
-        <v>0.246969979520418</v>
+        <v>0.537168623441823</v>
       </c>
       <c r="P54">
-        <v>8.37511</v>
+        <v>7.60852</v>
       </c>
       <c r="Q54">
         <v>0.2697</v>
@@ -4477,52 +4477,52 @@
     </row>
     <row r="55" spans="1:23">
       <c r="A55" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B55">
-        <v>1521494</v>
+        <v>1766823</v>
       </c>
       <c r="C55">
-        <v>446.49182222143</v>
+        <v>448.239009246395</v>
       </c>
       <c r="D55">
-        <v>4162.9027820022</v>
+        <v>4325.18565586736</v>
       </c>
       <c r="E55">
-        <v>0.124183006584644</v>
+        <v>0.146198824048042</v>
       </c>
       <c r="F55">
-        <v>3701.3876953125</v>
+        <v>3758.38061523438</v>
       </c>
       <c r="G55">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H55">
-        <v>0.118592367041856</v>
+        <v>0.214664444327354</v>
       </c>
       <c r="I55">
-        <v>0.118592367041856</v>
+        <v>0.214664444327354</v>
       </c>
       <c r="J55">
-        <v>0.117543860287633</v>
+        <v>0.0653333344872793</v>
       </c>
       <c r="K55">
         <v>0.0333333333333333</v>
       </c>
       <c r="L55">
-        <v>0.934640522875817</v>
+        <v>0.929824561403509</v>
       </c>
       <c r="M55">
-        <v>0.934640522875817</v>
+        <v>0.929824561403509</v>
       </c>
       <c r="N55">
-        <v>0.597967909477195</v>
+        <v>0.418282559234269</v>
       </c>
       <c r="O55">
-        <v>0.537168623441823</v>
+        <v>0.374656400314555</v>
       </c>
       <c r="P55">
-        <v>7.60852</v>
+        <v>9.14733</v>
       </c>
       <c r="Q55">
         <v>0.2697</v>
@@ -4548,52 +4548,52 @@
     </row>
     <row r="56" spans="1:23">
       <c r="A56" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B56">
-        <v>1766823</v>
+        <v>1338446</v>
       </c>
       <c r="C56">
-        <v>453.366776904471</v>
+        <v>454.96370360312</v>
       </c>
       <c r="D56">
-        <v>4324.3076135049</v>
+        <v>4703.30829497795</v>
       </c>
       <c r="E56">
-        <v>0.146198824048042</v>
+        <v>0.209150329232216</v>
       </c>
       <c r="F56">
-        <v>3758.38061523438</v>
+        <v>3814.765625</v>
       </c>
       <c r="G56">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H56">
-        <v>0.214664444327354</v>
+        <v>0.236223973333836</v>
       </c>
       <c r="I56">
-        <v>0.214664444327354</v>
+        <v>0.236223973333836</v>
       </c>
       <c r="J56">
-        <v>0.0653333344872793</v>
+        <v>0.095833334957327</v>
       </c>
       <c r="K56">
         <v>0.0333333333333333</v>
       </c>
       <c r="L56">
-        <v>0.929824561403509</v>
+        <v>0.862745098039216</v>
       </c>
       <c r="M56">
-        <v>0.929824561403509</v>
+        <v>0.862745098039216</v>
       </c>
       <c r="N56">
-        <v>0.418282559234269</v>
+        <v>0.564743071624211</v>
       </c>
       <c r="O56">
-        <v>0.374656400314555</v>
+        <v>0.501152761560821</v>
       </c>
       <c r="P56">
-        <v>9.14733</v>
+        <v>11.8862</v>
       </c>
       <c r="Q56">
         <v>0.2697</v>
@@ -4619,52 +4619,52 @@
     </row>
     <row r="57" spans="1:23">
       <c r="A57" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B57">
-        <v>1338446</v>
+        <v>1067173</v>
       </c>
       <c r="C57">
-        <v>460.168400465307</v>
+        <v>371.939687697328</v>
       </c>
       <c r="D57">
-        <v>4701.93184620075</v>
+        <v>4024.75253068253</v>
       </c>
       <c r="E57">
-        <v>0.209150329232216</v>
+        <v>0.248062014579773</v>
       </c>
       <c r="F57">
-        <v>3814.765625</v>
+        <v>3118.62841796875</v>
       </c>
       <c r="G57">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H57">
-        <v>0.236223973333836</v>
+        <v>0.163533758372068</v>
       </c>
       <c r="I57">
-        <v>0.236223973333836</v>
+        <v>0.163533758372068</v>
       </c>
       <c r="J57">
-        <v>0.095833334957327</v>
+        <v>0.108333334730317</v>
       </c>
       <c r="K57">
         <v>0.0333333333333333</v>
       </c>
       <c r="L57">
-        <v>0.862745098039216</v>
+        <v>0.868217054263566</v>
       </c>
       <c r="M57">
-        <v>0.862745098039216</v>
+        <v>0.868217054263566</v>
       </c>
       <c r="N57">
-        <v>0.564743071624211</v>
+        <v>0.604311997744502</v>
       </c>
       <c r="O57">
-        <v>0.501152761560821</v>
+        <v>0.532744940274463</v>
       </c>
       <c r="P57">
-        <v>11.8862</v>
+        <v>6.50645</v>
       </c>
       <c r="Q57">
         <v>0.2697</v>
@@ -4690,52 +4690,52 @@
     </row>
     <row r="58" spans="1:23">
       <c r="A58" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B58">
-        <v>1067173</v>
+        <v>1094013</v>
       </c>
       <c r="C58">
-        <v>376.19460585926</v>
+        <v>429.717965314139</v>
       </c>
       <c r="D58">
-        <v>4023.3488463474</v>
+        <v>4104.14405566194</v>
       </c>
       <c r="E58">
-        <v>0.248062014579773</v>
+        <v>0.136363640427589</v>
       </c>
       <c r="F58">
-        <v>3118.62841796875</v>
+        <v>3603.0859375</v>
       </c>
       <c r="G58">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H58">
-        <v>0.163533758372068</v>
+        <v>0.291658207774162</v>
       </c>
       <c r="I58">
-        <v>0.163533758372068</v>
+        <v>0.291658207774162</v>
       </c>
       <c r="J58">
-        <v>0.108333334730317</v>
+        <v>0.100000001490116</v>
       </c>
       <c r="K58">
         <v>0.0333333333333333</v>
       </c>
       <c r="L58">
-        <v>0.868217054263566</v>
+        <v>0.909090909090909</v>
       </c>
       <c r="M58">
-        <v>0.868217054263566</v>
+        <v>0.909090909090909</v>
       </c>
       <c r="N58">
-        <v>0.604311997744502</v>
+        <v>0.467809867931872</v>
       </c>
       <c r="O58">
-        <v>0.532744940274463</v>
+        <v>0.419573740971629</v>
       </c>
       <c r="P58">
-        <v>6.50645</v>
+        <v>11.3891</v>
       </c>
       <c r="Q58">
         <v>0.2697</v>
@@ -4761,52 +4761,52 @@
     </row>
     <row r="59" spans="1:23">
       <c r="A59" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B59">
-        <v>1094013</v>
+        <v>1795403</v>
       </c>
       <c r="C59">
-        <v>434.633855808223</v>
+        <v>402.231574577114</v>
       </c>
       <c r="D59">
-        <v>4103.36786239925</v>
+        <v>4044.75031844069</v>
       </c>
       <c r="E59">
-        <v>0.136363640427589</v>
+        <v>0.184523805975914</v>
       </c>
       <c r="F59">
-        <v>3603.0859375</v>
+        <v>3372.61889648438</v>
       </c>
       <c r="G59">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H59">
-        <v>0.291658207774162</v>
+        <v>0.259860575199127</v>
       </c>
       <c r="I59">
-        <v>0.291658207774162</v>
+        <v>0.259860575199127</v>
       </c>
       <c r="J59">
-        <v>0.100000001490116</v>
+        <v>0.07204301387635</v>
       </c>
       <c r="K59">
         <v>0.0333333333333333</v>
       </c>
       <c r="L59">
-        <v>0.909090909090909</v>
+        <v>0.922619047619048</v>
       </c>
       <c r="M59">
-        <v>0.909090909090909</v>
+        <v>0.922619047619048</v>
       </c>
       <c r="N59">
-        <v>0.467809867931872</v>
+        <v>0.308074783670659</v>
       </c>
       <c r="O59">
-        <v>0.419573740971629</v>
+        <v>0.274433013928521</v>
       </c>
       <c r="P59">
-        <v>11.3891</v>
+        <v>7.24176</v>
       </c>
       <c r="Q59">
         <v>0.2697</v>
@@ -4832,52 +4832,52 @@
     </row>
     <row r="60" spans="1:23">
       <c r="A60" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B60">
-        <v>1795403</v>
+        <v>2278114</v>
       </c>
       <c r="C60">
-        <v>406.833026072023</v>
+        <v>412.323697055793</v>
       </c>
       <c r="D60">
-        <v>4043.70911411237</v>
+        <v>4163.01408409867</v>
       </c>
       <c r="E60">
-        <v>0.184523805975914</v>
+        <v>0.188172042369843</v>
       </c>
       <c r="F60">
-        <v>3372.61889648438</v>
+        <v>3457.23901367188</v>
       </c>
       <c r="G60">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H60">
-        <v>0.259860575199127</v>
+        <v>0.197066821157932</v>
       </c>
       <c r="I60">
-        <v>0.259860575199127</v>
+        <v>0.197066821157932</v>
       </c>
       <c r="J60">
-        <v>0.07204301387635</v>
+        <v>0.0504761902791302</v>
       </c>
       <c r="K60">
         <v>0.0333333333333333</v>
       </c>
       <c r="L60">
-        <v>0.922619047619048</v>
+        <v>0.875675675675676</v>
       </c>
       <c r="M60">
-        <v>0.922619047619048</v>
+        <v>0.875675675675676</v>
       </c>
       <c r="N60">
-        <v>0.308074783670659</v>
+        <v>0.428289720847899</v>
       </c>
       <c r="O60">
-        <v>0.274433013928521</v>
+        <v>0.381310304502141</v>
       </c>
       <c r="P60">
-        <v>7.24176</v>
+        <v>8.68129</v>
       </c>
       <c r="Q60">
         <v>0.2697</v>
@@ -4903,52 +4903,52 @@
     </row>
     <row r="61" spans="1:23">
       <c r="A61" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B61">
-        <v>2278114</v>
+        <v>1776300</v>
       </c>
       <c r="C61">
-        <v>417.040600481882</v>
+        <v>477.608115241961</v>
       </c>
       <c r="D61">
-        <v>4161.92076211708</v>
+        <v>5489.69724639451</v>
       </c>
       <c r="E61">
-        <v>0.188172042369843</v>
+        <v>0.296296298503876</v>
       </c>
       <c r="F61">
-        <v>3457.23901367188</v>
+        <v>4004.6337890625</v>
       </c>
       <c r="G61">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H61">
-        <v>0.197066821157932</v>
+        <v>0.218547604978085</v>
       </c>
       <c r="I61">
-        <v>0.197066821157932</v>
+        <v>0.218547604978085</v>
       </c>
       <c r="J61">
-        <v>0.0504761902791302</v>
+        <v>0.0958333321691801</v>
       </c>
       <c r="K61">
         <v>0.0333333333333333</v>
       </c>
       <c r="L61">
-        <v>0.875675675675676</v>
+        <v>0.895061728395062</v>
       </c>
       <c r="M61">
-        <v>0.875675675675676</v>
+        <v>0.895061728395062</v>
       </c>
       <c r="N61">
-        <v>0.428289720847899</v>
+        <v>0.477331921865745</v>
       </c>
       <c r="O61">
-        <v>0.381310304502141</v>
+        <v>0.416928072932213</v>
       </c>
       <c r="P61">
-        <v>8.68129</v>
+        <v>7.33588</v>
       </c>
       <c r="Q61">
         <v>0.2697</v>
@@ -4974,52 +4974,52 @@
     </row>
     <row r="62" spans="1:23">
       <c r="A62" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B62">
-        <v>1776300</v>
+        <v>1249838</v>
       </c>
       <c r="C62">
-        <v>483.071859797995</v>
+        <v>476.609862691329</v>
       </c>
       <c r="D62">
-        <v>5487.39672234656</v>
+        <v>5102.44059908821</v>
       </c>
       <c r="E62">
-        <v>0.296296298503876</v>
+        <v>0.239130437374115</v>
       </c>
       <c r="F62">
-        <v>4004.6337890625</v>
+        <v>3996.263671875</v>
       </c>
       <c r="G62">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H62">
-        <v>0.218547604978085</v>
+        <v>0.174407631158829</v>
       </c>
       <c r="I62">
-        <v>0.218547604978085</v>
+        <v>0.174407631158829</v>
       </c>
       <c r="J62">
-        <v>0.0958333321691801</v>
+        <v>0.0393939393169706</v>
       </c>
       <c r="K62">
         <v>0.0333333333333333</v>
       </c>
       <c r="L62">
-        <v>0.895061728395062</v>
+        <v>0.927536231884058</v>
       </c>
       <c r="M62">
-        <v>0.895061728395062</v>
+        <v>0.927536231884058</v>
       </c>
       <c r="N62">
-        <v>0.477331921865745</v>
+        <v>0.386586392911113</v>
       </c>
       <c r="O62">
-        <v>0.416928072932213</v>
+        <v>0.341341421140387</v>
       </c>
       <c r="P62">
-        <v>7.33588</v>
+        <v>7.01821</v>
       </c>
       <c r="Q62">
         <v>0.2697</v>
@@ -5045,52 +5045,52 @@
     </row>
     <row r="63" spans="1:23">
       <c r="A63" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B63">
-        <v>1249838</v>
+        <v>826311</v>
       </c>
       <c r="C63">
-        <v>482.062187431065</v>
+        <v>456.868577016807</v>
       </c>
       <c r="D63">
-        <v>5100.72701128846</v>
+        <v>5731.50874962999</v>
       </c>
       <c r="E63">
-        <v>0.239130437374115</v>
+        <v>0.360360354185104</v>
       </c>
       <c r="F63">
-        <v>3996.263671875</v>
+        <v>3830.73754882812</v>
       </c>
       <c r="G63">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H63">
-        <v>0.174407631158829</v>
+        <v>0.28019779920578</v>
       </c>
       <c r="I63">
-        <v>0.174407631158829</v>
+        <v>0.28019779920578</v>
       </c>
       <c r="J63">
-        <v>0.0393939393169706</v>
+        <v>0.11833333700647</v>
       </c>
       <c r="K63">
         <v>0.0333333333333333</v>
       </c>
       <c r="L63">
-        <v>0.927536231884058</v>
+        <v>0.899082568807339</v>
       </c>
       <c r="M63">
-        <v>0.927536231884058</v>
+        <v>0.899082568807339</v>
       </c>
       <c r="N63">
-        <v>0.386586392911113</v>
+        <v>0.459386012985998</v>
       </c>
       <c r="O63">
-        <v>0.341341421140387</v>
+        <v>0.395430739115401</v>
       </c>
       <c r="P63">
-        <v>7.01821</v>
+        <v>8.54887</v>
       </c>
       <c r="Q63">
         <v>0.2697</v>
@@ -5116,52 +5116,52 @@
     </row>
     <row r="64" spans="1:23">
       <c r="A64" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B64">
-        <v>826311</v>
+        <v>1369152</v>
       </c>
       <c r="C64">
-        <v>462.095065262792</v>
+        <v>361.977864488398</v>
       </c>
       <c r="D64">
-        <v>5728.5642492886</v>
+        <v>4211.27491658273</v>
       </c>
       <c r="E64">
-        <v>0.360360354185104</v>
+        <v>0.305555552244186</v>
       </c>
       <c r="F64">
-        <v>3830.73754882812</v>
+        <v>3035.10083007812</v>
       </c>
       <c r="G64">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H64">
-        <v>0.28019779920578</v>
+        <v>0.21113008633256</v>
       </c>
       <c r="I64">
-        <v>0.28019779920578</v>
+        <v>0.21113008633256</v>
       </c>
       <c r="J64">
-        <v>0.11833333700647</v>
+        <v>0.106060609219406</v>
       </c>
       <c r="K64">
         <v>0.0333333333333333</v>
       </c>
       <c r="L64">
-        <v>0.899082568807339</v>
+        <v>0.798611111111111</v>
       </c>
       <c r="M64">
-        <v>0.899082568807339</v>
+        <v>0.798611111111111</v>
       </c>
       <c r="N64">
-        <v>0.459386012985998</v>
+        <v>0.609894007626845</v>
       </c>
       <c r="O64">
-        <v>0.395430739115401</v>
+        <v>0.531686071450096</v>
       </c>
       <c r="P64">
-        <v>8.54887</v>
+        <v>8.14925</v>
       </c>
       <c r="Q64">
         <v>0.2697</v>
@@ -5187,52 +5187,52 @@
     </row>
     <row r="65" spans="1:23">
       <c r="A65" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B65">
-        <v>1369152</v>
+        <v>910395</v>
       </c>
       <c r="C65">
-        <v>366.118821317621</v>
+        <v>381.894289851756</v>
       </c>
       <c r="D65">
-        <v>4209.4528956063</v>
+        <v>3596.92362601648</v>
       </c>
       <c r="E65">
-        <v>0.305555552244186</v>
+        <v>0.122807018458843</v>
       </c>
       <c r="F65">
-        <v>3035.10083007812</v>
+        <v>3202.09545898438</v>
       </c>
       <c r="G65">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H65">
-        <v>0.21113008633256</v>
+        <v>0.224404036998749</v>
       </c>
       <c r="I65">
-        <v>0.21113008633256</v>
+        <v>0.224404036998749</v>
       </c>
       <c r="J65">
-        <v>0.106060609219406</v>
+        <v>0.0904761887732007</v>
       </c>
       <c r="K65">
         <v>0.0333333333333333</v>
       </c>
       <c r="L65">
-        <v>0.798611111111111</v>
+        <v>0.929824561403509</v>
       </c>
       <c r="M65">
-        <v>0.798611111111111</v>
+        <v>0.929824561403509</v>
       </c>
       <c r="N65">
-        <v>0.609894007626845</v>
+        <v>0.827240503491187</v>
       </c>
       <c r="O65">
-        <v>0.531686071450096</v>
+        <v>0.743261520444602</v>
       </c>
       <c r="P65">
-        <v>8.14925</v>
+        <v>6.50645</v>
       </c>
       <c r="Q65">
         <v>0.2697</v>
@@ -5258,52 +5258,52 @@
     </row>
     <row r="66" spans="1:23">
       <c r="A66" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B66">
-        <v>910395</v>
+        <v>1285336</v>
       </c>
       <c r="C66">
-        <v>386.26308673893</v>
+        <v>358.764058477549</v>
       </c>
       <c r="D66">
-        <v>3596.31199444708</v>
+        <v>3682.54391149644</v>
       </c>
       <c r="E66">
-        <v>0.122807018458843</v>
+        <v>0.202898547053337</v>
       </c>
       <c r="F66">
-        <v>3202.09545898438</v>
+        <v>3008.15380859375</v>
       </c>
       <c r="G66">
-        <v>3692.17485218631</v>
+        <v>3707.47000281696</v>
       </c>
       <c r="H66">
-        <v>0.224404036998749</v>
+        <v>0.127139372751117</v>
       </c>
       <c r="I66">
-        <v>0.224404036998749</v>
+        <v>0.127139372751117</v>
       </c>
       <c r="J66">
-        <v>0.0904761887732007</v>
+        <v>0.133333332189137</v>
       </c>
       <c r="K66">
         <v>0.0333333333333333</v>
       </c>
       <c r="L66">
-        <v>0.929824561403509</v>
+        <v>0.934782608695652</v>
       </c>
       <c r="M66">
-        <v>0.929824561403509</v>
+        <v>0.934782608695652</v>
       </c>
       <c r="N66">
-        <v>0.827240503491187</v>
+        <v>0.698339528137324</v>
       </c>
       <c r="O66">
-        <v>0.743261520444602</v>
+        <v>0.620322932831807</v>
       </c>
       <c r="P66">
-        <v>6.50645</v>
+        <v>7.67476</v>
       </c>
       <c r="Q66">
         <v>0.2697</v>
@@ -5324,77 +5324,6 @@
         <v>1.5</v>
       </c>
       <c r="W66">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="67" spans="1:23">
-      <c r="A67" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B67">
-        <v>1285336</v>
-      </c>
-      <c r="C67">
-        <v>362.868249986972</v>
-      </c>
-      <c r="D67">
-        <v>3681.49920822684</v>
-      </c>
-      <c r="E67">
-        <v>0.202898547053337</v>
-      </c>
-      <c r="F67">
-        <v>3008.15380859375</v>
-      </c>
-      <c r="G67">
-        <v>3692.17485218631</v>
-      </c>
-      <c r="H67">
-        <v>0.127139372751117</v>
-      </c>
-      <c r="I67">
-        <v>0.127139372751117</v>
-      </c>
-      <c r="J67">
-        <v>0.133333332189137</v>
-      </c>
-      <c r="K67">
-        <v>0.0333333333333333</v>
-      </c>
-      <c r="L67">
-        <v>0.934782608695652</v>
-      </c>
-      <c r="M67">
-        <v>0.934782608695652</v>
-      </c>
-      <c r="N67">
-        <v>0.698339528137324</v>
-      </c>
-      <c r="O67">
-        <v>0.620322932831807</v>
-      </c>
-      <c r="P67">
-        <v>7.67476</v>
-      </c>
-      <c r="Q67">
-        <v>0.2697</v>
-      </c>
-      <c r="R67">
-        <v>3</v>
-      </c>
-      <c r="S67">
-        <v>0.2</v>
-      </c>
-      <c r="T67">
-        <v>0</v>
-      </c>
-      <c r="U67">
-        <v>0</v>
-      </c>
-      <c r="V67">
-        <v>1.5</v>
-      </c>
-      <c r="W67">
         <v>0.05</v>
       </c>
     </row>

</xml_diff>